<commit_message>
exp #3 ar ari swori
</commit_message>
<xml_diff>
--- a/ElectroMagnetismExperiments.xlsx
+++ b/ElectroMagnetismExperiments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University\PhysicsExperiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B8F9744-AA81-4027-86DF-1973D534F4C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB07680B-DB15-4692-837A-515A7E5E827B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{6671F666-8E3F-41E1-B59C-C232B66DC115}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <r>
       <rPr>
@@ -290,6 +290,15 @@
   <si>
     <t>tesla</t>
   </si>
+  <si>
+    <t xml:space="preserve">chveni b= </t>
+  </si>
+  <si>
+    <t>mashin N</t>
+  </si>
+  <si>
+    <t>:((((((</t>
+  </si>
 </sst>
 </file>
 
@@ -298,14 +307,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -468,10 +470,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -490,17 +499,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2329,8 +2331,8 @@
       <xdr:row>15</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4">
@@ -2402,6 +2404,7 @@
               </a:endParaRPr>
             </a:p>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -2437,7 +2440,7 @@
                                   <a:schemeClr val="dk1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -2450,7 +2453,7 @@
                                   <a:schemeClr val="dk1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -2464,7 +2467,7 @@
                                   <a:schemeClr val="dk1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -2478,7 +2481,7 @@
                               <a:schemeClr val="dk1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -2490,7 +2493,7 @@
                               <a:schemeClr val="dk1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -2504,7 +2507,7 @@
                                   <a:schemeClr val="dk1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -2520,7 +2523,7 @@
                                   <a:schemeClr val="dk1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -2536,7 +2539,7 @@
                                       <a:schemeClr val="dk1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="+mn-lt"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -2552,7 +2555,7 @@
                                       <a:schemeClr val="dk1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="+mn-lt"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -2566,7 +2569,7 @@
                                       <a:schemeClr val="dk1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="+mn-lt"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -2582,7 +2585,7 @@
                               <a:schemeClr val="dk1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -2596,7 +2599,7 @@
                                   <a:schemeClr val="dk1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -2612,7 +2615,7 @@
                                   <a:schemeClr val="dk1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -2628,7 +2631,7 @@
                                       <a:schemeClr val="dk1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="+mn-lt"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -2644,7 +2647,7 @@
                                       <a:schemeClr val="dk1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="+mn-lt"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -2658,7 +2661,7 @@
                                       <a:schemeClr val="dk1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="+mn-lt"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -2674,7 +2677,7 @@
                               <a:schemeClr val="dk1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -2704,7 +2707,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4">
@@ -3181,18 +3184,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
@@ -3200,20 +3203,20 @@
       <c r="O1" s="4"/>
     </row>
     <row r="3" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="D3" s="11" t="s">
+      <c r="B3" s="13"/>
+      <c r="D3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="12"/>
-      <c r="F3" s="13"/>
-      <c r="H3" s="11" t="s">
+      <c r="E3" s="15"/>
+      <c r="F3" s="16"/>
+      <c r="H3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="12"/>
-      <c r="J3" s="13"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="16"/>
     </row>
     <row r="4" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
@@ -3470,49 +3473,50 @@
   <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="H9" sqref="H8:H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.85546875" customWidth="1"/>
+    <col min="14" max="14" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="16"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="10"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="11" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
       <c r="G3" t="s">
         <v>30</v>
       </c>
@@ -3521,13 +3525,13 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="11" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="16"/>
+      <c r="C4" s="10"/>
       <c r="F4" t="s">
         <v>28</v>
       </c>
@@ -3541,59 +3545,75 @@
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="11" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="16"/>
+      <c r="C5" s="10"/>
+      <c r="M5" t="s">
+        <v>31</v>
+      </c>
+      <c r="N5">
+        <v>17</v>
+      </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="11" t="s">
         <v>18</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="16"/>
+      <c r="C6" s="10"/>
+      <c r="M6" t="s">
+        <v>32</v>
+      </c>
+      <c r="N6">
+        <f>(17*0.16)/((4*PI()*10^(-7))*0.37*COS(ATAN(1/2)))</f>
+        <v>6540520.669238925</v>
+      </c>
     </row>
     <row r="7" spans="1:15" ht="18.75" x14ac:dyDescent="0.35">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="12" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="16"/>
+      <c r="C7" s="10"/>
+      <c r="N7" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="8" spans="1:15" ht="18.75" x14ac:dyDescent="0.35">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="12" t="s">
         <v>20</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="16"/>
+      <c r="C8" s="10"/>
     </row>
     <row r="9" spans="1:15" ht="18.75" x14ac:dyDescent="0.35">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="12" t="s">
         <v>22</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="16"/>
+      <c r="C9" s="10"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="E10" s="16"/>
+      <c r="E10" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:O1"/>
     <mergeCell ref="A2:B2"/>
   </mergeCells>
-  <phoneticPr fontId="9" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
n = 600 :(
</commit_message>
<xml_diff>
--- a/ElectroMagnetismExperiments.xlsx
+++ b/ElectroMagnetismExperiments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University\PhysicsExperiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB07680B-DB15-4692-837A-515A7E5E827B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF1A265-6A02-442F-941C-30BC5EEB69B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{6671F666-8E3F-41E1-B59C-C232B66DC115}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <r>
       <rPr>
@@ -298,6 +298,12 @@
   </si>
   <si>
     <t>:((((((</t>
+  </si>
+  <si>
+    <t>(bruni)</t>
+  </si>
+  <si>
+    <t>(gauss)</t>
   </si>
 </sst>
 </file>
@@ -3473,7 +3479,7 @@
   <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H8:H9"/>
+      <selection activeCell="O32" sqref="O32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3558,6 +3564,9 @@
       <c r="N5">
         <v>17</v>
       </c>
+      <c r="O5" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
@@ -3571,8 +3580,11 @@
         <v>32</v>
       </c>
       <c r="N6">
-        <f>(17*0.16)/((4*PI()*10^(-7))*0.37*COS(ATAN(1/2)))</f>
-        <v>6540520.669238925</v>
+        <f>((17*10^(-4))*0.16)/((4*PI()*10^(-7))*0.37*COS(ATAN(1/2)))</f>
+        <v>654.05206692389254</v>
+      </c>
+      <c r="O6" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="18.75" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
swori zomebit mainc 600 bruni unda
</commit_message>
<xml_diff>
--- a/ElectroMagnetismExperiments.xlsx
+++ b/ElectroMagnetismExperiments.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University\PhysicsExperiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF1A265-6A02-442F-941C-30BC5EEB69B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57985AF6-1D38-4537-A7B3-3017A229C23D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{6671F666-8E3F-41E1-B59C-C232B66DC115}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6671F666-8E3F-41E1-B59C-C232B66DC115}"/>
   </bookViews>
   <sheets>
     <sheet name="I" sheetId="1" r:id="rId1"/>
     <sheet name="II" sheetId="2" r:id="rId2"/>
     <sheet name="III" sheetId="3" r:id="rId3"/>
+    <sheet name="IV" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
   <si>
     <r>
       <rPr>
@@ -213,32 +214,6 @@
   </si>
   <si>
     <r>
-      <t>tan</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(1/2)</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>µ</t>
     </r>
     <r>
@@ -270,12 +245,6 @@
     </r>
   </si>
   <si>
-    <t>0.16 მ</t>
-  </si>
-  <si>
-    <t>0.08 მ</t>
-  </si>
-  <si>
     <t>200 ბრუნი</t>
   </si>
   <si>
@@ -291,19 +260,48 @@
     <t>tesla</t>
   </si>
   <si>
-    <t xml:space="preserve">chveni b= </t>
-  </si>
-  <si>
     <t>mashin N</t>
-  </si>
-  <si>
-    <t>:((((((</t>
   </si>
   <si>
     <t>(bruni)</t>
   </si>
   <si>
     <t>(gauss)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chveni b </t>
+  </si>
+  <si>
+    <t>0.15 მ</t>
+  </si>
+  <si>
+    <t>0.06 მ</t>
+  </si>
+  <si>
+    <r>
+      <t>tan</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(3/7.5)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -453,7 +451,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -486,6 +484,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3179,8 +3180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A047B489-A731-456E-8B69-90BDAD212723}">
   <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3190,18 +3191,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
@@ -3209,20 +3210,20 @@
       <c r="O1" s="4"/>
     </row>
     <row r="3" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="D3" s="14" t="s">
+      <c r="B3" s="14"/>
+      <c r="D3" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="15"/>
-      <c r="F3" s="16"/>
-      <c r="H3" s="14" t="s">
+      <c r="E3" s="16"/>
+      <c r="F3" s="17"/>
+      <c r="H3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="15"/>
-      <c r="J3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="17"/>
     </row>
     <row r="4" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
@@ -3476,10 +3477,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{084737F5-A16E-4044-B5A7-1D23C9BBB711}">
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:O31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O32" sqref="O32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3489,29 +3490,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="20"/>
+      <c r="B2" s="21"/>
       <c r="C2" s="10"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -3519,106 +3520,111 @@
         <v>14</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
-      <c r="G3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="C4" s="10"/>
-      <c r="F4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4">
-        <f>((4*PI()*10^(-7))*200*0.37*(2*COS(ATAN(1/2))))/0.32</f>
-        <v>5.1983629009701377E-4</v>
-      </c>
-      <c r="H4">
-        <f>G4*10^4</f>
-        <v>5.198362900970138</v>
-      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C5" s="10"/>
-      <c r="M5" t="s">
-        <v>31</v>
-      </c>
-      <c r="N5">
-        <v>17</v>
-      </c>
-      <c r="O5" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>18</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C6" s="10"/>
-      <c r="M6" t="s">
-        <v>32</v>
-      </c>
-      <c r="N6">
-        <f>((17*10^(-4))*0.16)/((4*PI()*10^(-7))*0.37*COS(ATAN(1/2)))</f>
-        <v>654.05206692389254</v>
-      </c>
-      <c r="O6" t="s">
-        <v>34</v>
-      </c>
     </row>
     <row r="7" spans="1:15" ht="18.75" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="C7" s="10"/>
-      <c r="N7" t="s">
-        <v>33</v>
-      </c>
     </row>
     <row r="8" spans="1:15" ht="18.75" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
         <v>20</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="C8" s="10"/>
     </row>
     <row r="9" spans="1:15" ht="18.75" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="C9" s="10"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E10" s="10"/>
+    </row>
+    <row r="25" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="L25" t="s">
+        <v>27</v>
+      </c>
+      <c r="M25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K26" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="L26">
+        <f>((4*PI()*10^(-7))*200*0.37*(2*COS(ATAN(3/7.5))))/0.3</f>
+        <v>5.7560072208659311E-4</v>
+      </c>
+      <c r="M26">
+        <f>L26*10^4</f>
+        <v>5.7560072208659312</v>
+      </c>
+    </row>
+    <row r="30" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K30" t="s">
+        <v>31</v>
+      </c>
+      <c r="L30">
+        <v>17</v>
+      </c>
+      <c r="M30" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K31" t="s">
+        <v>28</v>
+      </c>
+      <c r="L31">
+        <f>((17*10^(-4))*0.16)/((4*PI()*10^(-7))*0.37*COS(ATAN(3/7.5)))</f>
+        <v>630.06638586549127</v>
+      </c>
+      <c r="M31" t="s">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3627,7 +3633,21 @@
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43B60A86-33F5-4671-9BE2-C9B2FA4F67DD}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
III eqsperimenti (solenoidi) gaformda
</commit_message>
<xml_diff>
--- a/ElectroMagnetismExperiments.xlsx
+++ b/ElectroMagnetismExperiments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University\PhysicsExperiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{641C5D13-7F5F-42A2-8F4E-C8D9CE655D48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87B13C53-03CC-4508-9770-3FDBE0ADC26A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{6671F666-8E3F-41E1-B59C-C232B66DC115}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{6671F666-8E3F-41E1-B59C-C232B66DC115}"/>
   </bookViews>
   <sheets>
     <sheet name="I" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="41">
   <si>
     <r>
       <rPr>
@@ -245,31 +245,7 @@
     </r>
   </si>
   <si>
-    <t>200 ბრუნი</t>
-  </si>
-  <si>
     <t>0.37 ა</t>
-  </si>
-  <si>
-    <t>B=</t>
-  </si>
-  <si>
-    <t>gauss</t>
-  </si>
-  <si>
-    <t>tesla</t>
-  </si>
-  <si>
-    <t>mashin N</t>
-  </si>
-  <si>
-    <t>(bruni)</t>
-  </si>
-  <si>
-    <t>(gauss)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chveni b </t>
   </si>
   <si>
     <t>0.15 მ</t>
@@ -416,6 +392,28 @@
   <si>
     <t>% ცდომილება:</t>
   </si>
+  <si>
+    <t>600 ხ</t>
+  </si>
+  <si>
+    <r>
+      <t>B</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>max</t>
+    </r>
+  </si>
+  <si>
+    <t>17 გ</t>
+  </si>
 </sst>
 </file>
 
@@ -423,16 +421,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -600,7 +591,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -623,7 +614,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -641,6 +632,23 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -667,25 +675,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2452,23 +2446,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>551898</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>588226</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4110F97-1151-434C-BA76-DA5C11CD477D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2C3D6DE-7D78-4924-A5DD-40A929F8C35B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2489,9 +2483,9 @@
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="3448050"/>
-          <a:ext cx="3104598" cy="1819275"/>
+        <a:xfrm rot="5400000">
+          <a:off x="1694288" y="2220487"/>
+          <a:ext cx="8429625" cy="3988651"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2500,21 +2494,26 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4">
@@ -2528,7 +2527,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="0" y="2295525"/>
+              <a:off x="0" y="3409950"/>
               <a:ext cx="2847975" cy="1019175"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -2889,7 +2888,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4">
@@ -2903,7 +2902,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="0" y="2295525"/>
+              <a:off x="0" y="3409950"/>
               <a:ext cx="2847975" cy="1019175"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -2961,71 +2960,12 @@
               </a:endParaRPr>
             </a:p>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-US" sz="1400" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
                 <a:t>𝐵=(</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1400" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="dk1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>𝜇_0 𝑁𝐼(cos⁡〖</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="el-GR" sz="1400" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="dk1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>Θ</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1400" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="dk1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>_1 〗+cos⁡〖</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="el-GR" sz="1400" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="dk1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>Θ</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1400" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="dk1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>_2 〗)</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-US" sz="1400" b="0" i="0">
@@ -3037,13 +2977,638 @@
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>)/</a:t>
+                <a:t>𝜇_0 𝑁𝐼(cos⁡〖</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="el-GR" sz="1400" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>Θ</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1400" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>_1 〗+cos⁡〖</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="el-GR" sz="1400" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>Θ</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1400" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>_2 〗))/</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-US" sz="1400" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
                 <a:t>2𝐿</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1400"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>368872</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>933449</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65BE05DB-E9D5-4066-9D4C-D1D9A8B8394A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2921572" y="933450"/>
+          <a:ext cx="6050977" cy="3562350"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="8" name="TextBox 7">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18AB0C81-A267-43AD-B6F6-D92A177F9FF7}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="904875" y="5172075"/>
+              <a:ext cx="7000875" cy="838200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:ln w="9525" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝐵</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>4</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝜋</m:t>
+                        </m:r>
+                        <m:sSup>
+                          <m:sSupPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSupPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>10</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sup>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>−7</m:t>
+                            </m:r>
+                          </m:sup>
+                        </m:sSup>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>∗600∗0.37∗2</m:t>
+                        </m:r>
+                        <m:func>
+                          <m:funcPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:funcPr>
+                          <m:fName>
+                            <m:r>
+                              <m:rPr>
+                                <m:sty m:val="p"/>
+                              </m:rPr>
+                              <a:rPr lang="en-US" sz="1400" b="0" i="0">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>cos</m:t>
+                            </m:r>
+                          </m:fName>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>(</m:t>
+                            </m:r>
+                            <m:func>
+                              <m:funcPr>
+                                <m:ctrlPr>
+                                  <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:funcPr>
+                              <m:fName>
+                                <m:sSup>
+                                  <m:sSupPr>
+                                    <m:ctrlPr>
+                                      <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                      </a:rPr>
+                                    </m:ctrlPr>
+                                  </m:sSupPr>
+                                  <m:e>
+                                    <m:r>
+                                      <m:rPr>
+                                        <m:sty m:val="p"/>
+                                      </m:rPr>
+                                      <a:rPr lang="en-US" sz="1400" b="0" i="0">
+                                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                      </a:rPr>
+                                      <m:t>tan</m:t>
+                                    </m:r>
+                                  </m:e>
+                                  <m:sup>
+                                    <m:r>
+                                      <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                      </a:rPr>
+                                      <m:t>−1</m:t>
+                                    </m:r>
+                                  </m:sup>
+                                </m:sSup>
+                              </m:fName>
+                              <m:e>
+                                <m:f>
+                                  <m:fPr>
+                                    <m:ctrlPr>
+                                      <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                      </a:rPr>
+                                    </m:ctrlPr>
+                                  </m:fPr>
+                                  <m:num>
+                                    <m:r>
+                                      <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                      </a:rPr>
+                                      <m:t>3</m:t>
+                                    </m:r>
+                                  </m:num>
+                                  <m:den>
+                                    <m:r>
+                                      <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                      </a:rPr>
+                                      <m:t>7.5</m:t>
+                                    </m:r>
+                                  </m:den>
+                                </m:f>
+                              </m:e>
+                            </m:func>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>)</m:t>
+                            </m:r>
+                          </m:e>
+                        </m:func>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2∗0.15</m:t>
+                        </m:r>
+                      </m:den>
+                    </m:f>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:r>
+                      <m:rPr>
+                        <m:nor/>
+                      </m:rPr>
+                      <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike">
+                        <a:solidFill>
+                          <a:schemeClr val="dk1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>0.001727(</m:t>
+                    </m:r>
+                    <m:r>
+                      <m:rPr>
+                        <m:nor/>
+                      </m:rPr>
+                      <a:rPr lang="ka-GE" sz="1400" b="0" i="0" u="none" strike="noStrike">
+                        <a:solidFill>
+                          <a:schemeClr val="dk1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>ტესლა</m:t>
+                    </m:r>
+                    <m:r>
+                      <m:rPr>
+                        <m:nor/>
+                      </m:rPr>
+                      <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike">
+                        <a:solidFill>
+                          <a:schemeClr val="dk1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>)</m:t>
+                    </m:r>
+                    <m:r>
+                      <m:rPr>
+                        <m:nor/>
+                      </m:rPr>
+                      <a:rPr lang="ka-GE" sz="1400" b="0" i="0" u="none" strike="noStrike">
+                        <a:solidFill>
+                          <a:schemeClr val="dk1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t> = </m:t>
+                    </m:r>
+                    <m:r>
+                      <m:rPr>
+                        <m:nor/>
+                      </m:rPr>
+                      <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike">
+                        <a:solidFill>
+                          <a:schemeClr val="dk1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>17.26802</m:t>
+                    </m:r>
+                    <m:r>
+                      <m:rPr>
+                        <m:nor/>
+                      </m:rPr>
+                      <a:rPr lang="en-US" sz="1400"/>
+                      <m:t> </m:t>
+                    </m:r>
+                    <m:r>
+                      <m:rPr>
+                        <m:nor/>
+                      </m:rPr>
+                      <a:rPr lang="ka-GE" sz="1400" b="0" i="0"/>
+                      <m:t>(გაუსი)</m:t>
+                    </m:r>
+                    <m:r>
+                      <m:rPr>
+                        <m:nor/>
+                      </m:rPr>
+                      <a:rPr lang="en-US" sz="1400"/>
+                      <m:t> </m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1400"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="8" name="TextBox 7">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18AB0C81-A267-43AD-B6F6-D92A177F9FF7}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="904875" y="5172075"/>
+              <a:ext cx="7000875" cy="838200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:ln w="9525" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝐵=(4</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝜋10^(−7)∗600∗0.37∗2 cos⁡〖(tan^(−1)⁡〖3/7.5〗)〗)/(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>2∗0.15)=</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>"0.001727(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1400" b="0" i="0" u="none" strike="noStrike">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>ტესლა</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>)</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1400" b="0" i="0" u="none" strike="noStrike">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t> = </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>17.26802</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1400" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t> </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>(გაუსი)</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1400" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t> </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1400" i="0"/>
+                <a:t>"</a:t>
               </a:r>
               <a:endParaRPr lang="en-US" sz="1400"/>
             </a:p>
@@ -3056,7 +3621,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -3238,8 +3803,8 @@
       <xdr:row>13</xdr:row>
       <xdr:rowOff>114301</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7">
@@ -3346,7 +3911,7 @@
                               <a:schemeClr val="dk1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -3359,7 +3924,7 @@
                               <a:schemeClr val="dk1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -3401,7 +3966,7 @@
                               <a:schemeClr val="dk1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -3414,7 +3979,7 @@
                               <a:schemeClr val="dk1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -3444,7 +4009,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7">
@@ -3569,8 +4134,8 @@
       <xdr:row>13</xdr:row>
       <xdr:rowOff>28576</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="TextBox 8">
@@ -3646,7 +4211,7 @@
                               <a:schemeClr val="dk1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -3659,7 +4224,7 @@
                               <a:schemeClr val="dk1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -3673,7 +4238,7 @@
                               <a:schemeClr val="dk1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -3701,7 +4266,7 @@
                               <a:schemeClr val="dk1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -3714,7 +4279,7 @@
                               <a:schemeClr val="dk1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -3756,7 +4321,7 @@
                               <a:schemeClr val="dk1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -3769,7 +4334,7 @@
                               <a:schemeClr val="dk1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -3799,7 +4364,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="TextBox 8">
@@ -3948,8 +4513,8 @@
       <xdr:row>12</xdr:row>
       <xdr:rowOff>142876</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="TextBox 9">
@@ -4021,7 +4586,7 @@
                             <a:schemeClr val="dk1"/>
                           </a:solidFill>
                           <a:effectLst/>
-                          <a:latin typeface="+mn-lt"/>
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           <a:ea typeface="+mn-ea"/>
                           <a:cs typeface="+mn-cs"/>
                         </a:rPr>
@@ -4034,7 +4599,7 @@
                             <a:schemeClr val="dk1"/>
                           </a:solidFill>
                           <a:effectLst/>
-                          <a:latin typeface="+mn-lt"/>
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           <a:ea typeface="+mn-ea"/>
                           <a:cs typeface="+mn-cs"/>
                         </a:rPr>
@@ -4048,7 +4613,7 @@
                             <a:schemeClr val="dk1"/>
                           </a:solidFill>
                           <a:effectLst/>
-                          <a:latin typeface="+mn-lt"/>
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           <a:ea typeface="+mn-ea"/>
                           <a:cs typeface="+mn-cs"/>
                         </a:rPr>
@@ -4072,7 +4637,7 @@
                             <a:schemeClr val="dk1"/>
                           </a:solidFill>
                           <a:effectLst/>
-                          <a:latin typeface="+mn-lt"/>
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           <a:ea typeface="+mn-ea"/>
                           <a:cs typeface="+mn-cs"/>
                         </a:rPr>
@@ -4085,7 +4650,7 @@
                             <a:schemeClr val="dk1"/>
                           </a:solidFill>
                           <a:effectLst/>
-                          <a:latin typeface="+mn-lt"/>
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           <a:ea typeface="+mn-ea"/>
                           <a:cs typeface="+mn-cs"/>
                         </a:rPr>
@@ -4127,7 +4692,7 @@
                             <a:schemeClr val="dk1"/>
                           </a:solidFill>
                           <a:effectLst/>
-                          <a:latin typeface="+mn-lt"/>
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           <a:ea typeface="+mn-ea"/>
                           <a:cs typeface="+mn-cs"/>
                         </a:rPr>
@@ -4140,7 +4705,7 @@
                             <a:schemeClr val="dk1"/>
                           </a:solidFill>
                           <a:effectLst/>
-                          <a:latin typeface="+mn-lt"/>
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           <a:ea typeface="+mn-ea"/>
                           <a:cs typeface="+mn-cs"/>
                         </a:rPr>
@@ -4154,7 +4719,7 @@
                             <a:schemeClr val="dk1"/>
                           </a:solidFill>
                           <a:effectLst/>
-                          <a:latin typeface="+mn-lt"/>
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           <a:ea typeface="+mn-ea"/>
                           <a:cs typeface="+mn-cs"/>
                         </a:rPr>
@@ -4178,7 +4743,7 @@
                             <a:schemeClr val="dk1"/>
                           </a:solidFill>
                           <a:effectLst/>
-                          <a:latin typeface="+mn-lt"/>
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           <a:ea typeface="+mn-ea"/>
                           <a:cs typeface="+mn-cs"/>
                         </a:rPr>
@@ -4191,7 +4756,7 @@
                             <a:schemeClr val="dk1"/>
                           </a:solidFill>
                           <a:effectLst/>
-                          <a:latin typeface="+mn-lt"/>
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           <a:ea typeface="+mn-ea"/>
                           <a:cs typeface="+mn-cs"/>
                         </a:rPr>
@@ -4220,7 +4785,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="TextBox 9">
@@ -4677,18 +5242,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
@@ -4696,20 +5261,20 @@
       <c r="O1" s="4"/>
     </row>
     <row r="3" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="D3" s="17" t="s">
+      <c r="B3" s="23"/>
+      <c r="D3" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="18"/>
-      <c r="F3" s="19"/>
-      <c r="H3" s="17" t="s">
+      <c r="E3" s="25"/>
+      <c r="F3" s="26"/>
+      <c r="H3" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="18"/>
-      <c r="J3" s="19"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="26"/>
     </row>
     <row r="4" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
@@ -4953,20 +5518,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7F57C43-2DDE-4B8C-A428-9607BE2E4181}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{084737F5-A16E-4044-B5A7-1D23C9BBB711}">
-  <dimension ref="A1:O31"/>
+  <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4976,148 +5545,111 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="23"/>
       <c r="C2" s="10"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="10"/>
+      <c r="B4" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="30"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="10"/>
+      <c r="B5" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="B6" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B7" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B8" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="10"/>
-    </row>
-    <row r="7" spans="1:15" ht="18.75" x14ac:dyDescent="0.35">
-      <c r="A7" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="10"/>
-    </row>
-    <row r="8" spans="1:15" ht="18.75" x14ac:dyDescent="0.35">
-      <c r="A8" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="10"/>
+      <c r="C8" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="9" spans="1:15" ht="18.75" x14ac:dyDescent="0.35">
-      <c r="A9" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="10"/>
+      <c r="B9" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="B10" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="E10" s="10"/>
     </row>
-    <row r="25" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="L25" t="s">
-        <v>27</v>
-      </c>
-      <c r="M25" t="s">
-        <v>26</v>
+    <row r="11" spans="1:15" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="B11" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="26" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K26" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="L26">
-        <f>((4*PI()*10^(-7))*200*0.37*(2*COS(ATAN(3/7.5))))/0.3</f>
-        <v>5.7560072208659311E-4</v>
-      </c>
-      <c r="M26">
-        <f>L26*10^4</f>
-        <v>5.7560072208659312</v>
+    <row r="12" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+      <c r="B12" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
-    <row r="30" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K30" t="s">
-        <v>31</v>
-      </c>
-      <c r="L30">
-        <v>17</v>
-      </c>
-      <c r="M30" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K31" t="s">
-        <v>28</v>
-      </c>
-      <c r="L31">
-        <f>((17*10^(-4))*0.16)/((4*PI()*10^(-7))*0.37*COS(ATAN(3/7.5)))</f>
-        <v>630.06638586549127</v>
-      </c>
-      <c r="M31" t="s">
-        <v>29</v>
-      </c>
+    <row r="26" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K26" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:O1"/>
-    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="B4:C4"/>
   </mergeCells>
-  <phoneticPr fontId="9" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -5128,8 +5660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43B60A86-33F5-4671-9BE2-C9B2FA4F67DD}">
   <dimension ref="A1:Q10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:Q1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="V11" sqref="V11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5148,69 +5680,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="24"/>
+      <c r="A1" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="H4" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="I4" s="25"/>
-      <c r="J4" s="25"/>
-      <c r="N4" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="O4" s="25"/>
-      <c r="P4" s="25"/>
+      <c r="A4" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="H4" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="N4" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="O4" s="31"/>
+      <c r="P4" s="31"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
       <c r="B5" s="14" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="H5" s="9"/>
       <c r="I5" s="14" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="J5" s="14" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="N5" s="9"/>
       <c r="O5" s="14" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="P5" s="14" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B6" s="9">
         <v>3.9</v>
@@ -5219,7 +5751,7 @@
         <v>4.9800000000000004</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="I6" s="9">
         <v>3.9</v>
@@ -5228,7 +5760,7 @@
         <v>7.92</v>
       </c>
       <c r="N6" s="9" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="O6" s="9">
         <v>3.9</v>
@@ -5239,7 +5771,7 @@
     </row>
     <row r="7" spans="1:17" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B7" s="9">
         <v>6.8</v>
@@ -5248,7 +5780,7 @@
         <v>2.85</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="I7" s="9">
         <v>6.8</v>
@@ -5257,7 +5789,7 @@
         <v>1.86</v>
       </c>
       <c r="N7" s="9" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="O7" s="9">
         <v>6.8</v>
@@ -5268,81 +5800,81 @@
     </row>
     <row r="8" spans="1:17" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" s="27">
+        <v>32</v>
+      </c>
+      <c r="B8" s="17">
         <v>10</v>
       </c>
-      <c r="C8" s="27">
+      <c r="C8" s="17">
         <v>1.96</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="I8" s="27">
+        <v>32</v>
+      </c>
+      <c r="I8" s="17">
         <v>10</v>
       </c>
-      <c r="J8" s="27">
+      <c r="J8" s="17">
         <v>1.86</v>
       </c>
       <c r="N8" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="O8" s="27">
+        <v>32</v>
+      </c>
+      <c r="O8" s="17">
         <v>10</v>
       </c>
-      <c r="P8" s="27">
+      <c r="P8" s="17">
         <v>9.84</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="26"/>
-      <c r="B9" s="28" t="s">
-        <v>44</v>
+      <c r="A9" s="16"/>
+      <c r="B9" s="18" t="s">
+        <v>36</v>
       </c>
       <c r="C9" s="15">
         <f>SUM(C6:C8)</f>
         <v>9.7899999999999991</v>
       </c>
-      <c r="H9" s="26"/>
-      <c r="I9" s="28" t="s">
-        <v>44</v>
+      <c r="H9" s="16"/>
+      <c r="I9" s="18" t="s">
+        <v>36</v>
       </c>
       <c r="J9" s="15">
         <f>(J6+J7)</f>
         <v>9.7799999999999994</v>
       </c>
-      <c r="N9" s="26"/>
-      <c r="O9" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="P9" s="29">
+      <c r="N9" s="16"/>
+      <c r="O9" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="P9" s="19">
         <f>AVERAGE(P6:P8)</f>
         <v>9.8366666666666678</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
-      <c r="B10" s="31" t="s">
-        <v>45</v>
+      <c r="A10" s="16"/>
+      <c r="B10" s="21" t="s">
+        <v>37</v>
       </c>
       <c r="C10" s="15">
         <f>(ABS((10-C9)/10)*100)</f>
         <v>2.1000000000000085</v>
       </c>
-      <c r="H10" s="26"/>
-      <c r="I10" s="31" t="s">
-        <v>45</v>
+      <c r="H10" s="16"/>
+      <c r="I10" s="21" t="s">
+        <v>37</v>
       </c>
       <c r="J10" s="15">
         <f>(ABS((10-J9)/10)*100)</f>
         <v>2.2000000000000064</v>
       </c>
-      <c r="N10" s="26"/>
-      <c r="O10" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="P10" s="30">
+      <c r="N10" s="16"/>
+      <c r="O10" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="P10" s="20">
         <f>(ABS((10-P9)/10)*100)</f>
         <v>1.633333333333322</v>
       </c>
@@ -5354,7 +5886,7 @@
     <mergeCell ref="N4:P4"/>
     <mergeCell ref="A1:Q1"/>
   </mergeCells>
-  <phoneticPr fontId="9" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
mexute damtavrebuli ar ari
</commit_message>
<xml_diff>
--- a/ElectroMagnetismExperiments.xlsx
+++ b/ElectroMagnetismExperiments.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University\PhysicsExperiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87B13C53-03CC-4508-9770-3FDBE0ADC26A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66725B95-5F1D-4A5F-AF0A-783450766C43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{6671F666-8E3F-41E1-B59C-C232B66DC115}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{6671F666-8E3F-41E1-B59C-C232B66DC115}"/>
   </bookViews>
   <sheets>
     <sheet name="I" sheetId="1" r:id="rId1"/>
     <sheet name="II" sheetId="2" r:id="rId2"/>
     <sheet name="III" sheetId="3" r:id="rId3"/>
     <sheet name="IV" sheetId="4" r:id="rId4"/>
+    <sheet name="V" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="46">
   <si>
     <r>
       <rPr>
@@ -414,14 +415,31 @@
   <si>
     <t>17 გ</t>
   </si>
+  <si>
+    <t>მიმდევრობითი/პარალელური შეერთების წრედები
+ექსპერიმენტი #6</t>
+  </si>
+  <si>
+    <t>R(Ω)</t>
+  </si>
+  <si>
+    <t>I(ა)</t>
+  </si>
+  <si>
+    <t>V(ვ)</t>
+  </si>
+  <si>
+    <t>გაზომვა</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="0.000000"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -514,7 +532,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -587,11 +605,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -680,6 +711,17 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2512,8 +2554,8 @@
       <xdr:row>20</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4">
@@ -2888,7 +2930,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4">
@@ -3104,8 +3146,8 @@
       <xdr:row>29</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7">
@@ -3154,6 +3196,7 @@
             <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -3460,7 +3503,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7">
@@ -4932,6 +4975,1284 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>98612</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Graphic 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E934C769-297F-4684-912B-88C287CF14D2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3603812" y="561975"/>
+          <a:ext cx="5463988" cy="4038600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>47626</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="12" name="TextBox 11">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30F912F3-6809-472A-A67D-2E7AD0C8FAFC}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="114300" y="609600"/>
+              <a:ext cx="3438526" cy="1409700"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:ln w="9525" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑅</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑉</m:t>
+                        </m:r>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝐼</m:t>
+                        </m:r>
+                      </m:den>
+                    </m:f>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1600" b="0"/>
+            </a:p>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝑅</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="ka-GE" sz="1600" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>მიმდევრობით</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="ka-GE" sz="1600" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="ka-GE" sz="1600" b="0" i="1"/>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑅</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>+</m:t>
+                    </m:r>
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="ka-GE" sz="1600" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝑅</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="dk1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>+…+</m:t>
+                    </m:r>
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="ka-GE" sz="1600" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝑅</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝑛</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1600"/>
+            </a:p>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="ka-GE" sz="1600" b="0" i="1"/>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1</m:t>
+                        </m:r>
+                      </m:num>
+                      <m:den>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1600" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="+mn-lt"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="+mn-lt"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>𝑅</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="ka-GE" sz="1600" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="+mn-lt"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>პარალელურად</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                      </m:den>
+                    </m:f>
+                    <m:r>
+                      <a:rPr lang="ka-GE" sz="1600" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="ka-GE" sz="1600" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>1</m:t>
+                        </m:r>
+                      </m:num>
+                      <m:den>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1600" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="+mn-lt"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="+mn-lt"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>𝑅</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>1</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                      </m:den>
+                    </m:f>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="dk1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>+</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="ka-GE" sz="1600" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>1</m:t>
+                        </m:r>
+                      </m:num>
+                      <m:den>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1600" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="+mn-lt"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="+mn-lt"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>𝑅</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>2</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                      </m:den>
+                    </m:f>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="dk1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>+…+</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="ka-GE" sz="1600" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>1</m:t>
+                        </m:r>
+                      </m:num>
+                      <m:den>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1600" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="+mn-lt"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="+mn-lt"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>𝑅</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>𝑛</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                      </m:den>
+                    </m:f>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1600"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="12" name="TextBox 11">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30F912F3-6809-472A-A67D-2E7AD0C8FAFC}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="114300" y="609600"/>
+              <a:ext cx="3438526" cy="1409700"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:ln w="9525" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1600" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑅=𝑉/𝐼</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1600" b="0"/>
+            </a:p>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1600" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝑅</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1600" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1600" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>მიმდევრობით=</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1600" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑅</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1600" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1600" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>1+</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1600" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝑅</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1600" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1600" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>2+…+</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1600" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝑅</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1600" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1600" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝑛</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1600"/>
+            </a:p>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1600" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>1</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1600" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>/</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1600" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝑅_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1600" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>პარალელურად </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1600" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>=</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1600" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>1</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1600" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>/</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1600" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝑅_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1600" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>1</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1600" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t> </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1600" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>+</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1600" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>1</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1600" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>/</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1600" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝑅_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1600" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>2</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1600" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t> </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1600" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>+…+</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1600" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>1</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1600" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>/</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1600" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝑅_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1600" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝑛</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1600" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t> </a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1600"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="13" name="TextBox 12">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{109B3370-6190-4F12-A4D8-E3DB64282DB5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="476250" y="4514850"/>
+              <a:ext cx="8343900" cy="1562100"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:ln w="9525" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="ka-GE" sz="1800" b="0" i="1"/>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1800" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑅</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="ka-GE" sz="1800" b="0" i="1"/>
+                          <m:t>ექ</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1050"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="13" name="TextBox 12">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{109B3370-6190-4F12-A4D8-E3DB64282DB5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="476250" y="4514850"/>
+              <a:ext cx="8343900" cy="1562100"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:ln w="9525" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1800" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑅</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1800" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1800" b="0" i="0"/>
+                <a:t>ექ</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1050"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -5534,13 +6855,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{084737F5-A16E-4044-B5A7-1D23C9BBB711}">
   <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.85546875" customWidth="1"/>
+    <col min="2" max="2" width="7" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
     <col min="14" max="14" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5891,4 +7213,139 @@
   <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A0BC8F6-3D81-4270-8CC2-113BF72AFF6F}">
+  <dimension ref="A1:S25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.85546875" customWidth="1"/>
+    <col min="2" max="2" width="2" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="4.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
+    </row>
+    <row r="6" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B14" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="30"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B15" s="9"/>
+      <c r="C15" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="36" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B16" s="9">
+        <v>1</v>
+      </c>
+      <c r="C16" s="9">
+        <v>1000</v>
+      </c>
+      <c r="D16" s="34">
+        <f>E16/C16</f>
+        <v>4.7000000000000002E-3</v>
+      </c>
+      <c r="E16" s="35">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="17" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B17" s="9">
+        <v>2</v>
+      </c>
+      <c r="C17" s="9">
+        <v>4700</v>
+      </c>
+      <c r="D17" s="34">
+        <f t="shared" ref="D17:D19" si="0">E17/C17</f>
+        <v>2.1765957446808512E-3</v>
+      </c>
+      <c r="E17" s="35">
+        <v>10.23</v>
+      </c>
+    </row>
+    <row r="18" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B18" s="9">
+        <v>3</v>
+      </c>
+      <c r="C18" s="9">
+        <v>2200</v>
+      </c>
+      <c r="D18" s="34">
+        <f t="shared" si="0"/>
+        <v>2.0818181818181816E-3</v>
+      </c>
+      <c r="E18" s="35">
+        <v>4.58</v>
+      </c>
+    </row>
+    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B19" s="9">
+        <v>4</v>
+      </c>
+      <c r="C19" s="9">
+        <v>2700</v>
+      </c>
+      <c r="D19" s="34">
+        <f t="shared" si="0"/>
+        <v>2.0851851851851851E-3</v>
+      </c>
+      <c r="E19" s="35">
+        <v>5.63</v>
+      </c>
+    </row>
+    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="S25">
+        <f>ABS((15-15.32)/15)*100</f>
+        <v>2.1333333333333355</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="B14:E14"/>
+  </mergeCells>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
VII morcha; II meore dasrulebuli ar ari jer
</commit_message>
<xml_diff>
--- a/ElectroMagnetismExperiments.xlsx
+++ b/ElectroMagnetismExperiments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University\PhysicsExperiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39596FEF-8D49-4876-8565-C11C0A968D3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E94F9583-CED9-458A-B633-131BE07F1F3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{6671F666-8E3F-41E1-B59C-C232B66DC115}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{6671F666-8E3F-41E1-B59C-C232B66DC115}"/>
   </bookViews>
   <sheets>
     <sheet name="I" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="IV" sheetId="4" r:id="rId4"/>
     <sheet name="V" sheetId="5" r:id="rId5"/>
     <sheet name="VI" sheetId="6" r:id="rId6"/>
+    <sheet name="VII" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="80">
   <si>
     <r>
       <rPr>
@@ -527,6 +528,283 @@
   <si>
     <t>4.5 გ</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Experiment #10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>RC Time Constants</t>
+    </r>
+  </si>
+  <si>
+    <t>ძაბვა (ვ)</t>
+  </si>
+  <si>
+    <t>დრო (წმ)</t>
+  </si>
+  <si>
+    <t>სმ</t>
+  </si>
+  <si>
+    <t>ვოლტი</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>12</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>23</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>34</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>45</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>56</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>67</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>25</t>
+    </r>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>0.5 სმ</t>
+  </si>
+  <si>
+    <t>10 ვ</t>
+  </si>
+  <si>
+    <t>8 სმ</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <r>
+      <t>8.99*10</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> მ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/კ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -537,7 +815,14 @@
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -746,7 +1031,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -769,7 +1054,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -800,7 +1085,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -815,6 +1100,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -848,12 +1139,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2617,54 +2915,2134 @@
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>588226</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="5" name="TextBox 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{336AAD72-B6B8-4D1C-92E1-3C9499A4349B}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="1447799"/>
+              <a:ext cx="1200150" cy="504826"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:ln w="9525" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
+                <a:defRPr/>
+              </a:pPr>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="dk1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>𝑉</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="dk1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>=2</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="dk1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>𝑘</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="dk1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>𝜆</m:t>
+                    </m:r>
+                    <m:func>
+                      <m:funcPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:funcPr>
+                      <m:fName>
+                        <m:r>
+                          <m:rPr>
+                            <m:sty m:val="p"/>
+                          </m:rPr>
+                          <a:rPr lang="en-US" sz="1400" b="0" i="0">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>ln</m:t>
+                        </m:r>
+                      </m:fName>
+                      <m:e>
+                        <m:f>
+                          <m:fPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="+mn-lt"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:fPr>
+                          <m:num>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="+mn-lt"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>𝑎</m:t>
+                            </m:r>
+                          </m:num>
+                          <m:den>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="+mn-lt"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>𝑏</m:t>
+                            </m:r>
+                          </m:den>
+                        </m:f>
+                      </m:e>
+                    </m:func>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1400">
+                <a:effectLst/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="5" name="TextBox 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{336AAD72-B6B8-4D1C-92E1-3C9499A4349B}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="1447799"/>
+              <a:ext cx="1200150" cy="504826"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:ln w="9525" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
+                <a:defRPr/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="1400" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝑉=2𝑘𝜆 ln⁡〖𝑎/𝑏〗</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1400">
+                <a:effectLst/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>371476</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="7" name="TextBox 6">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6BE360D8-13CC-4618-A528-BE593F9B3A46}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="1971675"/>
+              <a:ext cx="981076" cy="542925"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:ln w="9525" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝐸</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑘</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝜆</m:t>
+                        </m:r>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑟</m:t>
+                        </m:r>
+                      </m:den>
+                    </m:f>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1400"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="7" name="TextBox 6">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6BE360D8-13CC-4618-A528-BE593F9B3A46}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="1971675"/>
+              <a:ext cx="981076" cy="542925"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:ln w="9525" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝐸=2𝑘</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝜆/</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑟</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1400"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>561976</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>561976</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="8" name="TextBox 7">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FC00B66-B766-4BE5-86C3-D52DC59BAAA6}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2028826" y="2609850"/>
+              <a:ext cx="2438400" cy="457200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:ln w="9525" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝜆</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="ka-GE" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="ka-GE" sz="1100" b="0" i="1">
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <a:rPr lang="ka-GE" sz="1100" b="0" i="1">
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1</m:t>
+                        </m:r>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="ka-GE" sz="1100" b="0" i="1">
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>72∗</m:t>
+                        </m:r>
+                        <m:sSup>
+                          <m:sSupPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="ka-GE" sz="1100" b="0" i="1">
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSupPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="ka-GE" sz="1100" b="0" i="1">
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>10</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sup>
+                            <m:r>
+                              <a:rPr lang="ka-GE" sz="1100" b="0" i="1">
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>8</m:t>
+                            </m:r>
+                          </m:sup>
+                        </m:sSup>
+                        <m:r>
+                          <a:rPr lang="ka-GE" sz="1100" b="0" i="1">
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>∗</m:t>
+                        </m:r>
+                        <m:func>
+                          <m:funcPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:funcPr>
+                          <m:fName>
+                            <m:r>
+                              <m:rPr>
+                                <m:sty m:val="p"/>
+                              </m:rPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>ln</m:t>
+                            </m:r>
+                          </m:fName>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="ka-GE" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>2</m:t>
+                            </m:r>
+                          </m:e>
+                        </m:func>
+                      </m:den>
+                    </m:f>
+                    <m:r>
+                      <a:rPr lang="ka-GE" sz="1100" b="0" i="1">
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=2∗</m:t>
+                    </m:r>
+                    <m:sSup>
+                      <m:sSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="ka-GE" sz="1100" b="0" i="1">
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="ka-GE" sz="1100" b="0" i="1">
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>10</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="ka-GE" sz="1100" b="0" i="1">
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>−10</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSup>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="8" name="TextBox 7">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FC00B66-B766-4BE5-86C3-D52DC59BAAA6}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2028826" y="2609850"/>
+              <a:ext cx="2438400" cy="457200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:ln w="9525" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝜆</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>=</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1100" b="0" i="0">
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>1/(72∗10^8∗</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>ln⁡</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>2 )</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1100" b="0" i="0">
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>=2∗10^(−10)</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>142876</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>47626</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9" name="TextBox 8">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{528A311E-25CD-47B0-B608-8B433A64FA76}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1609726" y="3886199"/>
+              <a:ext cx="2343150" cy="495301"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:ln w="9525" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝐸</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="ka-GE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2∗9∗</m:t>
+                        </m:r>
+                        <m:sSup>
+                          <m:sSupPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSupPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>10</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sup>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>9</m:t>
+                            </m:r>
+                          </m:sup>
+                        </m:sSup>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>∗2∗</m:t>
+                        </m:r>
+                        <m:sSup>
+                          <m:sSupPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSupPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>10</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sup>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>−10</m:t>
+                            </m:r>
+                          </m:sup>
+                        </m:sSup>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:den>
+                    </m:f>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=1.8</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9" name="TextBox 8">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{528A311E-25CD-47B0-B608-8B433A64FA76}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1609726" y="3886199"/>
+              <a:ext cx="2343150" cy="495301"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:ln w="9525" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝐸_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>2</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>=(2∗9∗10^9∗2∗10^(−10))/2=1.8</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2C3D6DE-7D78-4924-A5DD-40A929F8C35B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm rot="5400000">
-          <a:off x="1694288" y="2220487"/>
-          <a:ext cx="8429625" cy="3988651"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10" name="TextBox 9">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C623A84-A6C8-4946-90A7-05C4B3DA11DE}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1543050" y="4610100"/>
+              <a:ext cx="2600325" cy="419100"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:ln w="9525" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
+                <a:defRPr/>
+              </a:pPr>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝐸</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>4</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="dk1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>2∗9∗</m:t>
+                        </m:r>
+                        <m:sSup>
+                          <m:sSupPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="+mn-lt"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSupPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="+mn-lt"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>10</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sup>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="+mn-lt"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>9</m:t>
+                            </m:r>
+                          </m:sup>
+                        </m:sSup>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>∗2∗</m:t>
+                        </m:r>
+                        <m:sSup>
+                          <m:sSupPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="+mn-lt"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSupPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="+mn-lt"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>10</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sup>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="+mn-lt"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>−10</m:t>
+                            </m:r>
+                          </m:sup>
+                        </m:sSup>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>4</m:t>
+                        </m:r>
+                      </m:den>
+                    </m:f>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="dk1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="dk1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>0</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="dk1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>.</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="dk1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>9</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US">
+                <a:effectLst/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10" name="TextBox 9">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C623A84-A6C8-4946-90A7-05C4B3DA11DE}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1543050" y="4610100"/>
+              <a:ext cx="2600325" cy="419100"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:ln w="9525" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
+                <a:defRPr/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝐸_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>4</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>=(2∗9∗10^9∗2∗10^(−10))/</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>4</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>=</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>0</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>.</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>9</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US">
+                <a:effectLst/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="11" name="TextBox 10">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3A11C97-2A6B-4D41-B3CF-DBC190806C6E}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1504950" y="5438775"/>
+              <a:ext cx="2600325" cy="419100"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:ln w="9525" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
+                <a:defRPr/>
+              </a:pPr>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝐸</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>6</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="dk1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>2∗9∗</m:t>
+                        </m:r>
+                        <m:sSup>
+                          <m:sSupPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="+mn-lt"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSupPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="+mn-lt"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>10</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sup>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="+mn-lt"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>9</m:t>
+                            </m:r>
+                          </m:sup>
+                        </m:sSup>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>∗2∗</m:t>
+                        </m:r>
+                        <m:sSup>
+                          <m:sSupPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="+mn-lt"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSupPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="+mn-lt"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>10</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sup>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="+mn-lt"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>−10</m:t>
+                            </m:r>
+                          </m:sup>
+                        </m:sSup>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>6</m:t>
+                        </m:r>
+                      </m:den>
+                    </m:f>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="dk1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="dk1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>0</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="dk1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>.</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="dk1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>6</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US">
+                <a:effectLst/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="11" name="TextBox 10">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3A11C97-2A6B-4D41-B3CF-DBC190806C6E}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1504950" y="5438775"/>
+              <a:ext cx="2600325" cy="419100"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:ln w="9525" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
+                <a:defRPr/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝐸_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>6</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>=(2∗9∗10^9∗2∗10^(−10))/</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>6</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>=</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>0</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>.</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>6</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US">
+                <a:effectLst/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -7003,8 +9381,8 @@
       <xdr:row>11</xdr:row>
       <xdr:rowOff>109744</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5">
@@ -7051,6 +9429,7 @@
             <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -7128,7 +9507,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5">
@@ -7248,6 +9627,100 @@
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>455800</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4160C6F-F613-4756-8CF7-77A073F38C18}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{BEBA8EAE-BF5A-486C-A8C5-ECC9F3942E4B}">
+              <a14:imgProps xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a14:imgLayer r:embed="rId2">
+                  <a14:imgEffect>
+                    <a14:brightnessContrast bright="40000" contrast="40000"/>
+                  </a14:imgEffect>
+                </a14:imgLayer>
+              </a14:imgProps>
+            </a:ext>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2133600" y="676275"/>
+          <a:ext cx="6856600" cy="5019675"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF">
+            <a:shade val="85000"/>
+          </a:srgbClr>
+        </a:solidFill>
+        <a:ln w="88900" cap="sq">
+          <a:solidFill>
+            <a:srgbClr val="FFFFFF"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="55000" dist="18000" dir="5400000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="40000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront"/>
+          <a:lightRig rig="twoPt" dir="t">
+            <a:rot lat="0" lon="0" rev="7200000"/>
+          </a:lightRig>
+        </a:scene3d>
+        <a:sp3d>
+          <a:bevelT w="25400" h="19050"/>
+          <a:contourClr>
+            <a:srgbClr val="FFFFFF"/>
+          </a:contourClr>
+        </a:sp3d>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -7565,18 +10038,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
@@ -7584,20 +10057,20 @@
       <c r="O1" s="4"/>
     </row>
     <row r="3" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="D3" s="29" t="s">
+      <c r="B3" s="30"/>
+      <c r="D3" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="30"/>
-      <c r="F3" s="31"/>
-      <c r="H3" s="29" t="s">
+      <c r="E3" s="32"/>
+      <c r="F3" s="33"/>
+      <c r="H3" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="30"/>
-      <c r="J3" s="31"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="33"/>
     </row>
     <row r="4" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
@@ -7839,16 +10312,152 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7F57C43-2DDE-4B8C-A428-9607BE2E4181}">
-  <dimension ref="A1"/>
+  <dimension ref="A4:O10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <cols>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="45" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="45" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="45"/>
+      <c r="D4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" t="s">
+        <v>66</v>
+      </c>
+      <c r="J4">
+        <v>1.3</v>
+      </c>
+      <c r="K4" s="45"/>
+      <c r="L4" s="45"/>
+      <c r="M4" s="45"/>
+      <c r="N4" s="45"/>
+      <c r="O4" s="45"/>
+    </row>
+    <row r="5" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>6</v>
+      </c>
+      <c r="I5" t="s">
+        <v>67</v>
+      </c>
+      <c r="J5">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>6.9</v>
+      </c>
+      <c r="I6" t="s">
+        <v>68</v>
+      </c>
+      <c r="J6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>7.5</v>
+      </c>
+      <c r="I7" t="s">
+        <v>69</v>
+      </c>
+      <c r="J7">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>8</v>
+      </c>
+      <c r="I8" t="s">
+        <v>70</v>
+      </c>
+      <c r="J8">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+      <c r="D9">
+        <v>6</v>
+      </c>
+      <c r="E9">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="I9" t="s">
+        <v>71</v>
+      </c>
+      <c r="J9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+      <c r="D10">
+        <v>7</v>
+      </c>
+      <c r="E10">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="I10" t="s">
+        <v>72</v>
+      </c>
+      <c r="J10">
+        <v>1.75</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="9" type="noConversion"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -7869,23 +10478,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
-      <c r="O1" s="33"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C2" s="10"/>
@@ -7895,10 +10504,10 @@
       <c r="D3" s="10"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="35"/>
+      <c r="C4" s="37"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B5" s="11" t="s">
@@ -7973,7 +10582,7 @@
     <mergeCell ref="A1:O1"/>
     <mergeCell ref="B4:C4"/>
   </mergeCells>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -8004,42 +10613,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="37"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
+      <c r="Q1" s="39"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="H4" s="36" t="s">
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="H4" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36"/>
-      <c r="N4" s="36" t="s">
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
+      <c r="N4" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="O4" s="36"/>
-      <c r="P4" s="36"/>
+      <c r="O4" s="38"/>
+      <c r="P4" s="38"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
@@ -8210,7 +10819,7 @@
     <mergeCell ref="N4:P4"/>
     <mergeCell ref="A1:Q1"/>
   </mergeCells>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -8236,34 +10845,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="37"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
+      <c r="Q1" s="39"/>
     </row>
     <row r="6" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B14" s="34" t="s">
+      <c r="B14" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="35"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="37"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B15" s="9"/>
@@ -8355,36 +10964,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEDC371A-9F67-4F3D-B8D5-1EC47F7296F2}">
   <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:15" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
-      <c r="O1" s="33"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="36"/>
+      <c r="B3" s="38"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
@@ -8412,7 +11021,7 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A7" s="40" t="s">
+      <c r="A7" s="28" t="s">
         <v>47</v>
       </c>
       <c r="B7" s="26" t="s">
@@ -8420,7 +11029,7 @@
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="40" t="s">
+      <c r="A8" s="28" t="s">
         <v>49</v>
       </c>
       <c r="B8" s="26">
@@ -8428,7 +11037,7 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="40" t="s">
+      <c r="A9" s="28" t="s">
         <v>50</v>
       </c>
       <c r="B9" s="26">
@@ -8437,10 +11046,10 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="36" t="s">
+      <c r="A12" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="B12" s="36"/>
+      <c r="B12" s="38"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
@@ -8484,4 +11093,262 @@
   <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D49D5AD0-7264-46D4-B59C-C56F06CBC265}">
+  <dimension ref="A1:O29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="10.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
+      <c r="O1" s="42"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="43" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="29">
+        <v>0</v>
+      </c>
+      <c r="B4" s="44">
+        <v>9.9499999999999993</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="29">
+        <v>20</v>
+      </c>
+      <c r="B5" s="44">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="29">
+        <v>40</v>
+      </c>
+      <c r="B6" s="44">
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="29">
+        <v>60</v>
+      </c>
+      <c r="B7" s="44">
+        <v>5.55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="29">
+        <v>80</v>
+      </c>
+      <c r="B8" s="44">
+        <v>4.42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="29">
+        <v>100</v>
+      </c>
+      <c r="B9" s="44">
+        <v>3.71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="29">
+        <v>120</v>
+      </c>
+      <c r="B10" s="44">
+        <v>3.05</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="29">
+        <v>140</v>
+      </c>
+      <c r="B11" s="44">
+        <v>2.5099999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="29">
+        <v>160</v>
+      </c>
+      <c r="B12" s="44">
+        <v>2.06</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="29">
+        <v>180</v>
+      </c>
+      <c r="B13" s="44">
+        <v>1.69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="29">
+        <v>200</v>
+      </c>
+      <c r="B14" s="44">
+        <v>1.39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="29">
+        <v>220</v>
+      </c>
+      <c r="B15" s="44">
+        <v>1.1399999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="29">
+        <v>240</v>
+      </c>
+      <c r="B16" s="44">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="29">
+        <v>260</v>
+      </c>
+      <c r="B17" s="44">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="29">
+        <v>280</v>
+      </c>
+      <c r="B18" s="44">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="29">
+        <v>300</v>
+      </c>
+      <c r="B19" s="44">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="29">
+        <v>320</v>
+      </c>
+      <c r="B20" s="44">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="29">
+        <v>340</v>
+      </c>
+      <c r="B21" s="44">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="29">
+        <v>360</v>
+      </c>
+      <c r="B22" s="44">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="29">
+        <v>380</v>
+      </c>
+      <c r="B23" s="44">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="29">
+        <v>400</v>
+      </c>
+      <c r="B24" s="44">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="29">
+        <v>420</v>
+      </c>
+      <c r="B25" s="44">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="29">
+        <v>440</v>
+      </c>
+      <c r="B26" s="44">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="29">
+        <v>460</v>
+      </c>
+      <c r="B27" s="44">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="29">
+        <v>480</v>
+      </c>
+      <c r="B28" s="44">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="29">
+        <v>500</v>
+      </c>
+      <c r="B29" s="44">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:O1"/>
+  </mergeCells>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
kvela eqsperimenti morcha wesit
</commit_message>
<xml_diff>
--- a/ElectroMagnetismExperiments.xlsx
+++ b/ElectroMagnetismExperiments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University\PhysicsExperiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E94F9583-CED9-458A-B633-131BE07F1F3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C1AC8F8-E615-44DE-BA4B-531E386F065C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{6671F666-8E3F-41E1-B59C-C232B66DC115}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{6671F666-8E3F-41E1-B59C-C232B66DC115}"/>
   </bookViews>
   <sheets>
     <sheet name="I" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="81">
   <si>
     <r>
       <rPr>
@@ -569,9 +569,6 @@
     <t>დრო (წმ)</t>
   </si>
   <si>
-    <t>სმ</t>
-  </si>
-  <si>
     <t>ვოლტი</t>
   </si>
   <si>
@@ -748,6 +745,25 @@
     <t>k</t>
   </si>
   <si>
+    <t>Experiment 2</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">სმ </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(ცენტრიდან)</t>
+    </r>
+  </si>
+  <si>
     <r>
       <t>8.99*10</t>
     </r>
@@ -762,48 +778,6 @@
       </rPr>
       <t>9</t>
     </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> მ</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>/კ</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
   </si>
 </sst>
 </file>
@@ -816,13 +790,6 @@
     <numFmt numFmtId="166" formatCode="0.000000"/>
   </numFmts>
   <fonts count="16" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -932,6 +899,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1031,7 +1006,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1054,7 +1029,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1085,7 +1060,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1100,12 +1075,22 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1139,19 +1124,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2917,16 +2902,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>104774</xdr:rowOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>170136</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>65689</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>111672</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
@@ -2943,8 +2928,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="0" y="1447799"/>
-              <a:ext cx="1200150" cy="504826"/>
+              <a:off x="610914" y="2403584"/>
+              <a:ext cx="2758965" cy="703536"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -3007,7 +2992,7 @@
                           <a:schemeClr val="dk1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -3019,7 +3004,7 @@
                           <a:schemeClr val="dk1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -3031,7 +3016,7 @@
                           <a:schemeClr val="dk1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -3043,7 +3028,7 @@
                           <a:schemeClr val="dk1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -3057,7 +3042,7 @@
                               <a:schemeClr val="dk1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -3073,7 +3058,7 @@
                               <a:schemeClr val="dk1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -3089,7 +3074,7 @@
                                   <a:schemeClr val="dk1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -3102,7 +3087,7 @@
                                   <a:schemeClr val="dk1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -3116,7 +3101,7 @@
                                   <a:schemeClr val="dk1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -3126,6 +3111,186 @@
                         </m:f>
                       </m:e>
                     </m:func>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="dk1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>    </m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="dk1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>⟺    </m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="dk1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>𝜆</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="dk1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝑉</m:t>
+                        </m:r>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝑘</m:t>
+                        </m:r>
+                        <m:func>
+                          <m:funcPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:funcPr>
+                          <m:fName>
+                            <m:r>
+                              <m:rPr>
+                                <m:sty m:val="p"/>
+                              </m:rPr>
+                              <a:rPr lang="en-US" sz="1400" b="0" i="0">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>ln</m:t>
+                            </m:r>
+                          </m:fName>
+                          <m:e>
+                            <m:f>
+                              <m:fPr>
+                                <m:ctrlPr>
+                                  <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                                    <a:solidFill>
+                                      <a:schemeClr val="dk1"/>
+                                    </a:solidFill>
+                                    <a:effectLst/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    <a:cs typeface="+mn-cs"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:fPr>
+                              <m:num>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                                    <a:solidFill>
+                                      <a:schemeClr val="dk1"/>
+                                    </a:solidFill>
+                                    <a:effectLst/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    <a:cs typeface="+mn-cs"/>
+                                  </a:rPr>
+                                  <m:t>𝑎</m:t>
+                                </m:r>
+                              </m:num>
+                              <m:den>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                                    <a:solidFill>
+                                      <a:schemeClr val="dk1"/>
+                                    </a:solidFill>
+                                    <a:effectLst/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    <a:cs typeface="+mn-cs"/>
+                                  </a:rPr>
+                                  <m:t>𝑏</m:t>
+                                </m:r>
+                              </m:den>
+                            </m:f>
+                          </m:e>
+                        </m:func>
+                      </m:den>
+                    </m:f>
                   </m:oMath>
                 </m:oMathPara>
               </a14:m>
@@ -3153,8 +3318,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="0" y="1447799"/>
-              <a:ext cx="1200150" cy="504826"/>
+              <a:off x="610914" y="2403584"/>
+              <a:ext cx="2758965" cy="703536"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -3211,11 +3376,23 @@
                     <a:schemeClr val="dk1"/>
                   </a:solidFill>
                   <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>𝑉=2𝑘𝜆 ln⁡〖𝑎/𝑏〗</a:t>
+                <a:t>𝑉=2𝑘𝜆 ln⁡〖𝑎/𝑏〗     </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1400" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>⟺    𝜆=𝑉/(2𝑘 ln⁡〖𝑎/𝑏〗 )</a:t>
               </a:r>
               <a:endParaRPr lang="en-US" sz="1400">
                 <a:effectLst/>
@@ -3232,16 +3409,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>129409</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>371476</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>123826</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>100834</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
@@ -3258,8 +3435,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="0" y="1971675"/>
-              <a:ext cx="981076" cy="542925"/>
+              <a:off x="610914" y="3315357"/>
+              <a:ext cx="984360" cy="542925"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -3293,6 +3470,7 @@
             <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -3371,8 +3549,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="0" y="1971675"/>
-              <a:ext cx="981076" cy="542925"/>
+              <a:off x="610914" y="3315357"/>
+              <a:ext cx="984360" cy="542925"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -3406,6 +3584,7 @@
             <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-US" sz="1400" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
@@ -3435,25 +3614,25 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>561976</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>391259</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>140676</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>561976</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>591354</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>45427</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="8" name="TextBox 7">
+            <xdr:cNvPr id="9" name="TextBox 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FC00B66-B766-4BE5-86C3-D52DC59BAAA6}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{528A311E-25CD-47B0-B608-8B433A64FA76}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3461,8 +3640,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="2028826" y="2609850"/>
-              <a:ext cx="2438400" cy="457200"/>
+              <a:off x="5505451" y="3694234"/>
+              <a:ext cx="3240768" cy="666751"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -3496,144 +3675,131 @@
             <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
                     <m:jc m:val="centerGroup"/>
                   </m:oMathParaPr>
                   <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1600" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝐸</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="ka-GE" sz="1600" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
                     <m:r>
-                      <a:rPr lang="en-US" sz="1100" i="1">
+                      <a:rPr lang="en-US" sz="1600" b="0" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>𝜆</m:t>
-                    </m:r>
-                    <m:r>
-                      <a:rPr lang="ka-GE" sz="1100" b="0" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
                       <m:t>=</m:t>
                     </m:r>
                     <m:f>
                       <m:fPr>
                         <m:ctrlPr>
-                          <a:rPr lang="ka-GE" sz="1100" b="0" i="1">
-                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
                       </m:fPr>
                       <m:num>
                         <m:r>
-                          <a:rPr lang="ka-GE" sz="1100" b="0" i="1">
-                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>1</m:t>
-                        </m:r>
-                      </m:num>
-                      <m:den>
-                        <m:r>
-                          <a:rPr lang="ka-GE" sz="1100" b="0" i="1">
-                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>72∗</m:t>
+                          <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2∗9∗</m:t>
                         </m:r>
                         <m:sSup>
                           <m:sSupPr>
                             <m:ctrlPr>
-                              <a:rPr lang="ka-GE" sz="1100" b="0" i="1">
-                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
                             </m:ctrlPr>
                           </m:sSupPr>
                           <m:e>
                             <m:r>
-                              <a:rPr lang="ka-GE" sz="1100" b="0" i="1">
-                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
                               <m:t>10</m:t>
                             </m:r>
                           </m:e>
                           <m:sup>
                             <m:r>
-                              <a:rPr lang="ka-GE" sz="1100" b="0" i="1">
-                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
-                              <m:t>8</m:t>
+                              <m:t>9</m:t>
                             </m:r>
                           </m:sup>
                         </m:sSup>
                         <m:r>
-                          <a:rPr lang="ka-GE" sz="1100" b="0" i="1">
-                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>∗</m:t>
+                          <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>∗2∗</m:t>
                         </m:r>
-                        <m:func>
-                          <m:funcPr>
+                        <m:sSup>
+                          <m:sSupPr>
                             <m:ctrlPr>
-                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                              <a:rPr lang="en-US" sz="1600" b="0" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
                             </m:ctrlPr>
-                          </m:funcPr>
-                          <m:fName>
-                            <m:r>
-                              <m:rPr>
-                                <m:sty m:val="p"/>
-                              </m:rPr>
-                              <a:rPr lang="en-US" sz="1100" b="0" i="0">
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                              </a:rPr>
-                              <m:t>ln</m:t>
-                            </m:r>
-                          </m:fName>
+                          </m:sSupPr>
                           <m:e>
                             <m:r>
-                              <a:rPr lang="ka-GE" sz="1100" b="0" i="1">
+                              <a:rPr lang="en-US" sz="1600" b="0" i="1">
                                 <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
-                              <m:t>2</m:t>
+                              <m:t>10</m:t>
                             </m:r>
                           </m:e>
-                        </m:func>
+                          <m:sup>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>−10</m:t>
+                            </m:r>
+                          </m:sup>
+                        </m:sSup>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
                       </m:den>
                     </m:f>
                     <m:r>
-                      <a:rPr lang="ka-GE" sz="1100" b="0" i="1">
-                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
-                      <m:t>=2∗</m:t>
+                      <m:t>=1.8</m:t>
                     </m:r>
-                    <m:sSup>
-                      <m:sSupPr>
-                        <m:ctrlPr>
-                          <a:rPr lang="ka-GE" sz="1100" b="0" i="1">
-                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                        </m:ctrlPr>
-                      </m:sSupPr>
-                      <m:e>
-                        <m:r>
-                          <a:rPr lang="ka-GE" sz="1100" b="0" i="1">
-                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>10</m:t>
-                        </m:r>
-                      </m:e>
-                      <m:sup>
-                        <m:r>
-                          <a:rPr lang="ka-GE" sz="1100" b="0" i="1">
-                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>−10</m:t>
-                        </m:r>
-                      </m:sup>
-                    </m:sSup>
                   </m:oMath>
                 </m:oMathPara>
               </a14:m>
@@ -3645,10 +3811,10 @@
       <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="8" name="TextBox 7">
+            <xdr:cNvPr id="9" name="TextBox 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FC00B66-B766-4BE5-86C3-D52DC59BAAA6}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{528A311E-25CD-47B0-B608-8B433A64FA76}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3656,8 +3822,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="2028826" y="2609850"/>
-              <a:ext cx="2438400" cy="457200"/>
+              <a:off x="5505451" y="3694234"/>
+              <a:ext cx="3240768" cy="666751"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -3691,45 +3857,24 @@
             <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
             <a:lstStyle/>
             <a:p>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100" i="0">
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1600" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>𝜆</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="ka-GE" sz="1100" b="0" i="0">
+                </a:rPr>
+                <a:t>𝐸_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1600" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>=</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="ka-GE" sz="1100" b="0" i="0">
-                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>1/(72∗10^8∗</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                </a:rPr>
+                <a:t>2</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1600" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>ln⁡</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="ka-GE" sz="1100" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>2 )</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="ka-GE" sz="1100" b="0" i="0">
-                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>=2∗10^(−10)</a:t>
+                </a:rPr>
+                <a:t>=(2∗9∗10^9∗2∗10^(−10))/2=1.8</a:t>
               </a:r>
               <a:endParaRPr lang="en-US" sz="1100"/>
             </a:p>
@@ -3741,286 +3886,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>142876</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>47624</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>387265</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>52493</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>47626</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="9" name="TextBox 8">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{528A311E-25CD-47B0-B608-8B433A64FA76}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="1609726" y="3886199"/>
-              <a:ext cx="2343150" cy="495301"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:schemeClr val="lt1"/>
-            </a:solidFill>
-            <a:ln w="9525" cmpd="sng">
-              <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:shade val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="dk1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a14:m>
-                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                  <m:oMathParaPr>
-                    <m:jc m:val="centerGroup"/>
-                  </m:oMathParaPr>
-                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                    <m:sSub>
-                      <m:sSubPr>
-                        <m:ctrlPr>
-                          <a:rPr lang="en-US" sz="1100" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                        </m:ctrlPr>
-                      </m:sSubPr>
-                      <m:e>
-                        <m:r>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝐸</m:t>
-                        </m:r>
-                      </m:e>
-                      <m:sub>
-                        <m:r>
-                          <a:rPr lang="ka-GE" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>2</m:t>
-                        </m:r>
-                      </m:sub>
-                    </m:sSub>
-                    <m:r>
-                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>=</m:t>
-                    </m:r>
-                    <m:f>
-                      <m:fPr>
-                        <m:ctrlPr>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                        </m:ctrlPr>
-                      </m:fPr>
-                      <m:num>
-                        <m:r>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>2∗9∗</m:t>
-                        </m:r>
-                        <m:sSup>
-                          <m:sSupPr>
-                            <m:ctrlPr>
-                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                              </a:rPr>
-                            </m:ctrlPr>
-                          </m:sSupPr>
-                          <m:e>
-                            <m:r>
-                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                              </a:rPr>
-                              <m:t>10</m:t>
-                            </m:r>
-                          </m:e>
-                          <m:sup>
-                            <m:r>
-                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                              </a:rPr>
-                              <m:t>9</m:t>
-                            </m:r>
-                          </m:sup>
-                        </m:sSup>
-                        <m:r>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>∗2∗</m:t>
-                        </m:r>
-                        <m:sSup>
-                          <m:sSupPr>
-                            <m:ctrlPr>
-                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                              </a:rPr>
-                            </m:ctrlPr>
-                          </m:sSupPr>
-                          <m:e>
-                            <m:r>
-                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                              </a:rPr>
-                              <m:t>10</m:t>
-                            </m:r>
-                          </m:e>
-                          <m:sup>
-                            <m:r>
-                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                              </a:rPr>
-                              <m:t>−10</m:t>
-                            </m:r>
-                          </m:sup>
-                        </m:sSup>
-                      </m:num>
-                      <m:den>
-                        <m:r>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>2</m:t>
-                        </m:r>
-                      </m:den>
-                    </m:f>
-                    <m:r>
-                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>=1.8</m:t>
-                    </m:r>
-                  </m:oMath>
-                </m:oMathPara>
-              </a14:m>
-              <a:endParaRPr lang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="9" name="TextBox 8">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{528A311E-25CD-47B0-B608-8B433A64FA76}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="1609726" y="3886199"/>
-              <a:ext cx="2343150" cy="495301"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:schemeClr val="lt1"/>
-            </a:solidFill>
-            <a:ln w="9525" cmpd="sng">
-              <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:shade val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="dk1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>𝐸_</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="ka-GE" sz="1100" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>2</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>=(2∗9∗10^9∗2∗10^(−10))/2=1.8</a:t>
-              </a:r>
-              <a:endParaRPr lang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>591354</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:rowOff>109644</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
@@ -4037,8 +3912,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="1543050" y="4610100"/>
-              <a:ext cx="2600325" cy="419100"/>
+              <a:off x="5501457" y="4368051"/>
+              <a:ext cx="3244762" cy="628651"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -4098,12 +3973,12 @@
                     <m:sSub>
                       <m:sSubPr>
                         <m:ctrlPr>
-                          <a:rPr lang="en-US" sz="1100" i="1">
+                          <a:rPr lang="en-US" sz="1600" i="1">
                             <a:solidFill>
                               <a:schemeClr val="dk1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -4111,12 +3986,12 @@
                       </m:sSubPr>
                       <m:e>
                         <m:r>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                          <a:rPr lang="en-US" sz="1600" b="0" i="1">
                             <a:solidFill>
                               <a:schemeClr val="dk1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -4125,7 +4000,7 @@
                       </m:e>
                       <m:sub>
                         <m:r>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                          <a:rPr lang="en-US" sz="1600" b="0" i="1">
                             <a:solidFill>
                               <a:schemeClr val="dk1"/>
                             </a:solidFill>
@@ -4139,12 +4014,12 @@
                       </m:sub>
                     </m:sSub>
                     <m:r>
-                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                      <a:rPr lang="en-US" sz="1600" b="0" i="1">
                         <a:solidFill>
                           <a:schemeClr val="dk1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -4153,12 +4028,12 @@
                     <m:f>
                       <m:fPr>
                         <m:ctrlPr>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                          <a:rPr lang="en-US" sz="1600" b="0" i="1">
                             <a:solidFill>
                               <a:schemeClr val="dk1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -4166,12 +4041,12 @@
                       </m:fPr>
                       <m:num>
                         <m:r>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                          <a:rPr lang="en-US" sz="1600" b="0" i="1">
                             <a:solidFill>
                               <a:schemeClr val="dk1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -4180,12 +4055,12 @@
                         <m:sSup>
                           <m:sSupPr>
                             <m:ctrlPr>
-                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                              <a:rPr lang="en-US" sz="1600" b="0" i="1">
                                 <a:solidFill>
                                   <a:schemeClr val="dk1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -4193,12 +4068,12 @@
                           </m:sSupPr>
                           <m:e>
                             <m:r>
-                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                              <a:rPr lang="en-US" sz="1600" b="0" i="1">
                                 <a:solidFill>
                                   <a:schemeClr val="dk1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -4207,12 +4082,12 @@
                           </m:e>
                           <m:sup>
                             <m:r>
-                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                              <a:rPr lang="en-US" sz="1600" b="0" i="1">
                                 <a:solidFill>
                                   <a:schemeClr val="dk1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -4221,12 +4096,12 @@
                           </m:sup>
                         </m:sSup>
                         <m:r>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                          <a:rPr lang="en-US" sz="1600" b="0" i="1">
                             <a:solidFill>
                               <a:schemeClr val="dk1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -4235,12 +4110,12 @@
                         <m:sSup>
                           <m:sSupPr>
                             <m:ctrlPr>
-                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                              <a:rPr lang="en-US" sz="1600" b="0" i="1">
                                 <a:solidFill>
                                   <a:schemeClr val="dk1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -4248,12 +4123,12 @@
                           </m:sSupPr>
                           <m:e>
                             <m:r>
-                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                              <a:rPr lang="en-US" sz="1600" b="0" i="1">
                                 <a:solidFill>
                                   <a:schemeClr val="dk1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -4262,12 +4137,12 @@
                           </m:e>
                           <m:sup>
                             <m:r>
-                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                              <a:rPr lang="en-US" sz="1600" b="0" i="1">
                                 <a:solidFill>
                                   <a:schemeClr val="dk1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -4278,7 +4153,7 @@
                       </m:num>
                       <m:den>
                         <m:r>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                          <a:rPr lang="en-US" sz="1600" b="0" i="1">
                             <a:solidFill>
                               <a:schemeClr val="dk1"/>
                             </a:solidFill>
@@ -4292,19 +4167,7 @@
                       </m:den>
                     </m:f>
                     <m:r>
-                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                        <a:solidFill>
-                          <a:schemeClr val="dk1"/>
-                        </a:solidFill>
-                        <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
-                        <a:ea typeface="+mn-ea"/>
-                        <a:cs typeface="+mn-cs"/>
-                      </a:rPr>
-                      <m:t>=</m:t>
-                    </m:r>
-                    <m:r>
-                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                      <a:rPr lang="en-US" sz="1600" b="0" i="1">
                         <a:solidFill>
                           <a:schemeClr val="dk1"/>
                         </a:solidFill>
@@ -4313,36 +4176,12 @@
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
-                      <m:t>0</m:t>
-                    </m:r>
-                    <m:r>
-                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                        <a:solidFill>
-                          <a:schemeClr val="dk1"/>
-                        </a:solidFill>
-                        <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
-                        <a:ea typeface="+mn-ea"/>
-                        <a:cs typeface="+mn-cs"/>
-                      </a:rPr>
-                      <m:t>.</m:t>
-                    </m:r>
-                    <m:r>
-                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                        <a:solidFill>
-                          <a:schemeClr val="dk1"/>
-                        </a:solidFill>
-                        <a:effectLst/>
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        <a:ea typeface="+mn-ea"/>
-                        <a:cs typeface="+mn-cs"/>
-                      </a:rPr>
-                      <m:t>9</m:t>
+                      <m:t>=0.9</m:t>
                     </m:r>
                   </m:oMath>
                 </m:oMathPara>
               </a14:m>
-              <a:endParaRPr lang="en-US">
+              <a:endParaRPr lang="en-US" sz="1600">
                 <a:effectLst/>
               </a:endParaRPr>
             </a:p>
@@ -4366,8 +4205,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="1543050" y="4610100"/>
-              <a:ext cx="2600325" cy="419100"/>
+              <a:off x="5501457" y="4368051"/>
+              <a:ext cx="3244762" cy="628651"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -4419,19 +4258,7 @@
                 <a:defRPr/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="dk1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>𝐸_</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                <a:rPr lang="en-US" sz="1600" b="0" i="0">
                   <a:solidFill>
                     <a:schemeClr val="dk1"/>
                   </a:solidFill>
@@ -4440,81 +4267,9 @@
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>4</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="dk1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>=(2∗9∗10^9∗2∗10^(−10))/</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="dk1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>4</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="dk1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>=</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="dk1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>0</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="dk1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>.</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="dk1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>9</a:t>
-              </a:r>
-              <a:endParaRPr lang="en-US">
+                <a:t>𝐸_4=(2∗9∗10^9∗2∗10^(−10))/4=0.9</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1600">
                 <a:effectLst/>
               </a:endParaRPr>
             </a:p>
@@ -4529,16 +4284,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>390028</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>114560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>597498</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>143135</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
@@ -4555,8 +4310,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="1504950" y="5438775"/>
-              <a:ext cx="2600325" cy="419100"/>
+              <a:off x="5504220" y="5001618"/>
+              <a:ext cx="3248143" cy="600075"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -4616,12 +4371,12 @@
                     <m:sSub>
                       <m:sSubPr>
                         <m:ctrlPr>
-                          <a:rPr lang="en-US" sz="1100" i="1">
+                          <a:rPr lang="en-US" sz="1600" i="1">
                             <a:solidFill>
                               <a:schemeClr val="dk1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -4629,12 +4384,12 @@
                       </m:sSubPr>
                       <m:e>
                         <m:r>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                          <a:rPr lang="en-US" sz="1600" b="0" i="1">
                             <a:solidFill>
                               <a:schemeClr val="dk1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -4643,7 +4398,7 @@
                       </m:e>
                       <m:sub>
                         <m:r>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                          <a:rPr lang="en-US" sz="1600" b="0" i="1">
                             <a:solidFill>
                               <a:schemeClr val="dk1"/>
                             </a:solidFill>
@@ -4657,12 +4412,12 @@
                       </m:sub>
                     </m:sSub>
                     <m:r>
-                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                      <a:rPr lang="en-US" sz="1600" b="0" i="1">
                         <a:solidFill>
                           <a:schemeClr val="dk1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -4671,12 +4426,12 @@
                     <m:f>
                       <m:fPr>
                         <m:ctrlPr>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                          <a:rPr lang="en-US" sz="1600" b="0" i="1">
                             <a:solidFill>
                               <a:schemeClr val="dk1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -4684,12 +4439,12 @@
                       </m:fPr>
                       <m:num>
                         <m:r>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                          <a:rPr lang="en-US" sz="1600" b="0" i="1">
                             <a:solidFill>
                               <a:schemeClr val="dk1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -4698,12 +4453,12 @@
                         <m:sSup>
                           <m:sSupPr>
                             <m:ctrlPr>
-                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                              <a:rPr lang="en-US" sz="1600" b="0" i="1">
                                 <a:solidFill>
                                   <a:schemeClr val="dk1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -4711,12 +4466,12 @@
                           </m:sSupPr>
                           <m:e>
                             <m:r>
-                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                              <a:rPr lang="en-US" sz="1600" b="0" i="1">
                                 <a:solidFill>
                                   <a:schemeClr val="dk1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -4725,12 +4480,12 @@
                           </m:e>
                           <m:sup>
                             <m:r>
-                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                              <a:rPr lang="en-US" sz="1600" b="0" i="1">
                                 <a:solidFill>
                                   <a:schemeClr val="dk1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -4739,12 +4494,12 @@
                           </m:sup>
                         </m:sSup>
                         <m:r>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                          <a:rPr lang="en-US" sz="1600" b="0" i="1">
                             <a:solidFill>
                               <a:schemeClr val="dk1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -4753,12 +4508,12 @@
                         <m:sSup>
                           <m:sSupPr>
                             <m:ctrlPr>
-                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                              <a:rPr lang="en-US" sz="1600" b="0" i="1">
                                 <a:solidFill>
                                   <a:schemeClr val="dk1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -4766,12 +4521,12 @@
                           </m:sSupPr>
                           <m:e>
                             <m:r>
-                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                              <a:rPr lang="en-US" sz="1600" b="0" i="1">
                                 <a:solidFill>
                                   <a:schemeClr val="dk1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -4780,12 +4535,12 @@
                           </m:e>
                           <m:sup>
                             <m:r>
-                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                              <a:rPr lang="en-US" sz="1600" b="0" i="1">
                                 <a:solidFill>
                                   <a:schemeClr val="dk1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -4796,7 +4551,7 @@
                       </m:num>
                       <m:den>
                         <m:r>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                          <a:rPr lang="en-US" sz="1600" b="0" i="1">
                             <a:solidFill>
                               <a:schemeClr val="dk1"/>
                             </a:solidFill>
@@ -4810,19 +4565,7 @@
                       </m:den>
                     </m:f>
                     <m:r>
-                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                        <a:solidFill>
-                          <a:schemeClr val="dk1"/>
-                        </a:solidFill>
-                        <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
-                        <a:ea typeface="+mn-ea"/>
-                        <a:cs typeface="+mn-cs"/>
-                      </a:rPr>
-                      <m:t>=</m:t>
-                    </m:r>
-                    <m:r>
-                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                      <a:rPr lang="en-US" sz="1600" b="0" i="1">
                         <a:solidFill>
                           <a:schemeClr val="dk1"/>
                         </a:solidFill>
@@ -4831,36 +4574,12 @@
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
-                      <m:t>0</m:t>
-                    </m:r>
-                    <m:r>
-                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                        <a:solidFill>
-                          <a:schemeClr val="dk1"/>
-                        </a:solidFill>
-                        <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
-                        <a:ea typeface="+mn-ea"/>
-                        <a:cs typeface="+mn-cs"/>
-                      </a:rPr>
-                      <m:t>.</m:t>
-                    </m:r>
-                    <m:r>
-                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                        <a:solidFill>
-                          <a:schemeClr val="dk1"/>
-                        </a:solidFill>
-                        <a:effectLst/>
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        <a:ea typeface="+mn-ea"/>
-                        <a:cs typeface="+mn-cs"/>
-                      </a:rPr>
-                      <m:t>6</m:t>
+                      <m:t>=0.6</m:t>
                     </m:r>
                   </m:oMath>
                 </m:oMathPara>
               </a14:m>
-              <a:endParaRPr lang="en-US">
+              <a:endParaRPr lang="en-US" sz="1600">
                 <a:effectLst/>
               </a:endParaRPr>
             </a:p>
@@ -4884,8 +4603,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="1504950" y="5438775"/>
-              <a:ext cx="2600325" cy="419100"/>
+              <a:off x="5504220" y="5001618"/>
+              <a:ext cx="3248143" cy="600075"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -4937,7 +4656,943 @@
                 <a:defRPr/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                <a:rPr lang="en-US" sz="1600" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝐸_6=(2∗9∗10^9∗2∗10^(−10))/6=0.6</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1600">
+                <a:effectLst/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>781707</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>98536</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="TextBox 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B925D81-9DD0-4885-A3C3-99FA74339196}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="610914" y="1773622"/>
+              <a:ext cx="781707" cy="558362"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:ln w="9525" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝐸</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <a:rPr lang="el-GR" sz="1400" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>∆</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="el-GR" sz="1400" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝜑</m:t>
+                        </m:r>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="el-GR" sz="1400" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>∆</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑥</m:t>
+                        </m:r>
+                      </m:den>
+                    </m:f>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1400"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="TextBox 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B925D81-9DD0-4885-A3C3-99FA74339196}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="610914" y="1773622"/>
+              <a:ext cx="781707" cy="558362"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:ln w="9525" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝐸=</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="el-GR" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>∆𝜑</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>/</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="el-GR" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>∆</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑥</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1400"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>7327</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>117231</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>29308</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3" name="TextBox 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BD89204-2CCF-4AC0-9E3F-3667568A5D64}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="615462" y="4051789"/>
+              <a:ext cx="3055326" cy="1817077"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:ln w="9525" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑉</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=2.89875∗</m:t>
+                    </m:r>
+                    <m:sSup>
+                      <m:sSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>10</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>9</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSup>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>∗</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝜆</m:t>
+                    </m:r>
+                    <m:func>
+                      <m:funcPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:funcPr>
+                      <m:fName>
+                        <m:r>
+                          <m:rPr>
+                            <m:sty m:val="p"/>
+                          </m:rPr>
+                          <a:rPr lang="en-US" sz="1400" b="0" i="0">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>ln</m:t>
+                        </m:r>
+                      </m:fName>
+                      <m:e>
+                        <m:f>
+                          <m:fPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:fPr>
+                          <m:num>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑎</m:t>
+                            </m:r>
+                          </m:num>
+                          <m:den>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑏</m:t>
+                            </m:r>
+                          </m:den>
+                        </m:f>
+                      </m:e>
+                    </m:func>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1400"/>
+            </a:p>
+            <a:p>
+              <a:endParaRPr lang="en-US" sz="1400"/>
+            </a:p>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>10=</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="dk1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>2.89875∗</m:t>
+                    </m:r>
+                    <m:sSup>
+                      <m:sSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>10</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>9</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSup>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="dk1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>∗</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="dk1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>𝜆</m:t>
+                    </m:r>
+                    <m:func>
+                      <m:funcPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:funcPr>
+                      <m:fName>
+                        <m:r>
+                          <m:rPr>
+                            <m:sty m:val="p"/>
+                          </m:rPr>
+                          <a:rPr lang="en-US" sz="1400" b="0" i="0">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>ln</m:t>
+                        </m:r>
+                      </m:fName>
+                      <m:e>
+                        <m:f>
+                          <m:fPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="+mn-lt"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:fPr>
+                          <m:num>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>8</m:t>
+                            </m:r>
+                          </m:num>
+                          <m:den>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>0.5</m:t>
+                            </m:r>
+                          </m:den>
+                        </m:f>
+                      </m:e>
+                    </m:func>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1400"/>
+            </a:p>
+            <a:p>
+              <a:endParaRPr lang="en-US" sz="1400"/>
+            </a:p>
+            <a:p>
+              <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
+                <a:defRPr/>
+              </a:pPr>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1400" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="dk1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>𝜆</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="ka-GE" sz="1400" b="0" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="dk1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="ka-GE" sz="1400" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <a:rPr lang="ka-GE" sz="1400" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>1</m:t>
+                        </m:r>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="ka-GE" sz="1400" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>72∗</m:t>
+                        </m:r>
+                        <m:sSup>
+                          <m:sSupPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="ka-GE" sz="1400" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="+mn-lt"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSupPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="ka-GE" sz="1400" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="+mn-lt"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>10</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sup>
+                            <m:r>
+                              <a:rPr lang="ka-GE" sz="1400" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="+mn-lt"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>8</m:t>
+                            </m:r>
+                          </m:sup>
+                        </m:sSup>
+                        <m:r>
+                          <a:rPr lang="ka-GE" sz="1400" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>∗</m:t>
+                        </m:r>
+                        <m:func>
+                          <m:funcPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="+mn-lt"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:funcPr>
+                          <m:fName>
+                            <m:r>
+                              <m:rPr>
+                                <m:sty m:val="p"/>
+                              </m:rPr>
+                              <a:rPr lang="en-US" sz="1400" b="0" i="0">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="+mn-lt"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>ln</m:t>
+                            </m:r>
+                          </m:fName>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="ka-GE" sz="1400" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="+mn-lt"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>2</m:t>
+                            </m:r>
+                          </m:e>
+                        </m:func>
+                      </m:den>
+                    </m:f>
+                    <m:r>
+                      <a:rPr lang="ka-GE" sz="1400" b="0" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="dk1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>=2∗</m:t>
+                    </m:r>
+                    <m:sSup>
+                      <m:sSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="ka-GE" sz="1400" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="ka-GE" sz="1400" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>10</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="ka-GE" sz="1400" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>−10</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSup>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1400">
+                <a:effectLst/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3" name="TextBox 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BD89204-2CCF-4AC0-9E3F-3667568A5D64}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="615462" y="4051789"/>
+              <a:ext cx="3055326" cy="1817077"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:ln w="9525" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑉=2.89875∗10^9∗</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝜆 ln⁡〖𝑎/𝑏〗</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1400"/>
+            </a:p>
+            <a:p>
+              <a:endParaRPr lang="en-US" sz="1400"/>
+            </a:p>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>10=</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1400" b="0" i="0">
                   <a:solidFill>
                     <a:schemeClr val="dk1"/>
                   </a:solidFill>
@@ -4946,10 +5601,10 @@
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>𝐸_</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                <a:t>2.89875∗10^9∗𝜆 ln⁡〖</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1400" b="0" i="0">
                   <a:solidFill>
                     <a:schemeClr val="dk1"/>
                   </a:solidFill>
@@ -4958,10 +5613,10 @@
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>6</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                <a:t>8</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1400" b="0" i="0">
                   <a:solidFill>
                     <a:schemeClr val="dk1"/>
                   </a:solidFill>
@@ -4970,10 +5625,10 @@
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>=(2∗9∗10^9∗2∗10^(−10))/</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                <a:t>/</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1400" b="0" i="0">
                   <a:solidFill>
                     <a:schemeClr val="dk1"/>
                   </a:solidFill>
@@ -4982,10 +5637,10 @@
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>6</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                <a:t>0.5</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1400" b="0" i="0">
                   <a:solidFill>
                     <a:schemeClr val="dk1"/>
                   </a:solidFill>
@@ -4994,22 +5649,33 @@
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>=</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="dk1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>0</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                <a:t>〗</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1400"/>
+            </a:p>
+            <a:p>
+              <a:endParaRPr lang="en-US" sz="1400"/>
+            </a:p>
+            <a:p>
+              <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
+                <a:defRPr/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="1400" i="0">
                   <a:solidFill>
                     <a:schemeClr val="dk1"/>
                   </a:solidFill>
@@ -5018,21 +5684,45 @@
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>.</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                <a:t>𝜆</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1400" b="0" i="0">
                   <a:solidFill>
                     <a:schemeClr val="dk1"/>
                   </a:solidFill>
                   <a:effectLst/>
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>6</a:t>
-              </a:r>
-              <a:endParaRPr lang="en-US">
+                <a:t>=1/(72∗10^8∗</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1400" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>ln⁡</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1400" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>2 )=2∗10^(−10)</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1400">
                 <a:effectLst/>
               </a:endParaRPr>
             </a:p>
@@ -10038,18 +10728,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
@@ -10057,20 +10747,20 @@
       <c r="O1" s="4"/>
     </row>
     <row r="3" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="D3" s="31" t="s">
+      <c r="B3" s="34"/>
+      <c r="D3" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="32"/>
-      <c r="F3" s="33"/>
-      <c r="H3" s="31" t="s">
+      <c r="E3" s="36"/>
+      <c r="F3" s="37"/>
+      <c r="H3" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="32"/>
-      <c r="J3" s="33"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="37"/>
     </row>
     <row r="4" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
@@ -10312,10 +11002,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7F57C43-2DDE-4B8C-A428-9607BE2E4181}">
-  <dimension ref="A4:O10"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+    <sheetView topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10323,141 +11013,158 @@
     <col min="2" max="2" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="45" t="s">
+    <row r="1" spans="1:15" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="47" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+    </row>
+    <row r="3" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+      <c r="B3" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="H3" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="L3" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B4" s="45" t="s">
+      <c r="M3" s="9">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="49" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="49" t="s">
+        <v>74</v>
+      </c>
+      <c r="F4" s="33"/>
+      <c r="G4" s="49">
+        <v>2</v>
+      </c>
+      <c r="H4" s="49">
+        <v>6</v>
+      </c>
+      <c r="K4" s="33"/>
+      <c r="L4" s="49" t="s">
+        <v>66</v>
+      </c>
+      <c r="M4" s="49">
+        <v>0.74</v>
+      </c>
+      <c r="N4" s="33"/>
+      <c r="O4" s="33"/>
+    </row>
+    <row r="5" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+      <c r="B5" s="49" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="45"/>
-      <c r="D4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" t="s">
-        <v>66</v>
-      </c>
-      <c r="J4">
-        <v>1.3</v>
-      </c>
-      <c r="K4" s="45"/>
-      <c r="L4" s="45"/>
-      <c r="M4" s="45"/>
-      <c r="N4" s="45"/>
-      <c r="O4" s="45"/>
+      <c r="G5" s="49">
+        <v>3</v>
+      </c>
+      <c r="H5" s="49">
+        <v>6.9</v>
+      </c>
+      <c r="L5" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="M5" s="49">
+        <v>0.5</v>
+      </c>
     </row>
-    <row r="5" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B5" t="s">
-        <v>75</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5">
+    <row r="6" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+      <c r="B6" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" s="49" t="s">
+        <v>80</v>
+      </c>
+      <c r="G6" s="49">
+        <v>4</v>
+      </c>
+      <c r="H6" s="49">
+        <v>7.5</v>
+      </c>
+      <c r="L6" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="M6" s="49">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+      <c r="G7" s="49">
+        <v>5</v>
+      </c>
+      <c r="H7" s="49">
+        <v>8</v>
+      </c>
+      <c r="L7" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="M7" s="49">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+      <c r="G8" s="49">
         <v>6</v>
       </c>
-      <c r="I5" t="s">
-        <v>67</v>
-      </c>
-      <c r="J5">
-        <v>0.74</v>
+      <c r="H8" s="49">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="L8" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="M8" s="49">
+        <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B6" t="s">
-        <v>77</v>
-      </c>
-      <c r="D6">
-        <v>3</v>
-      </c>
-      <c r="E6">
-        <v>6.9</v>
-      </c>
-      <c r="I6" t="s">
-        <v>68</v>
-      </c>
-      <c r="J6">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="18.75" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>78</v>
-      </c>
-      <c r="B7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D7">
-        <v>4</v>
-      </c>
-      <c r="E7">
-        <v>7.5</v>
-      </c>
-      <c r="I7" t="s">
-        <v>69</v>
-      </c>
-      <c r="J7">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="D8">
-        <v>5</v>
-      </c>
-      <c r="E8">
-        <v>8</v>
-      </c>
-      <c r="I8" t="s">
-        <v>70</v>
-      </c>
-      <c r="J8">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="D9">
-        <v>6</v>
-      </c>
-      <c r="E9">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="I9" t="s">
+    <row r="9" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+      <c r="G9" s="49">
+        <v>7</v>
+      </c>
+      <c r="H9" s="49">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="L9" s="49" t="s">
         <v>71</v>
       </c>
-      <c r="J9">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="D10">
-        <v>7</v>
-      </c>
-      <c r="E10">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="I10" t="s">
-        <v>72</v>
-      </c>
-      <c r="J10">
+      <c r="M9" s="49">
         <v>1.75</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="9" type="noConversion"/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:O1"/>
+  </mergeCells>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -10478,23 +11185,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C2" s="10"/>
@@ -10504,10 +11211,10 @@
       <c r="D3" s="10"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="37"/>
+      <c r="C4" s="41"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B5" s="11" t="s">
@@ -10582,7 +11289,7 @@
     <mergeCell ref="A1:O1"/>
     <mergeCell ref="B4:C4"/>
   </mergeCells>
-  <phoneticPr fontId="9" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -10613,42 +11320,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="39"/>
-      <c r="Q1" s="39"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
+      <c r="Q1" s="43"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="H4" s="38" t="s">
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="H4" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
-      <c r="N4" s="38" t="s">
+      <c r="I4" s="42"/>
+      <c r="J4" s="42"/>
+      <c r="N4" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="O4" s="38"/>
-      <c r="P4" s="38"/>
+      <c r="O4" s="42"/>
+      <c r="P4" s="42"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
@@ -10819,7 +11526,7 @@
     <mergeCell ref="N4:P4"/>
     <mergeCell ref="A1:Q1"/>
   </mergeCells>
-  <phoneticPr fontId="9" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -10845,34 +11552,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="39"/>
-      <c r="Q1" s="39"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
+      <c r="Q1" s="43"/>
     </row>
     <row r="6" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B14" s="36" t="s">
+      <c r="B14" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="40"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="37"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="41"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B15" s="9"/>
@@ -10964,36 +11671,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEDC371A-9F67-4F3D-B8D5-1EC47F7296F2}">
   <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:15" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="38"/>
+      <c r="B3" s="42"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
@@ -11046,10 +11753,10 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="38" t="s">
+      <c r="A12" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="B12" s="38"/>
+      <c r="B12" s="42"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
@@ -11090,7 +11797,7 @@
     <mergeCell ref="A12:B12"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -11099,8 +11806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D49D5AD0-7264-46D4-B59C-C56F06CBC265}">
   <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11109,29 +11816,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
-      <c r="M1" s="42"/>
-      <c r="N1" s="42"/>
-      <c r="O1" s="42"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="31" t="s">
         <v>61</v>
       </c>
     </row>
@@ -11139,7 +11846,7 @@
       <c r="A4" s="29">
         <v>0</v>
       </c>
-      <c r="B4" s="44">
+      <c r="B4" s="32">
         <v>9.9499999999999993</v>
       </c>
     </row>
@@ -11147,7 +11854,7 @@
       <c r="A5" s="29">
         <v>20</v>
       </c>
-      <c r="B5" s="44">
+      <c r="B5" s="32">
         <v>8.1999999999999993</v>
       </c>
     </row>
@@ -11155,7 +11862,7 @@
       <c r="A6" s="29">
         <v>40</v>
       </c>
-      <c r="B6" s="44">
+      <c r="B6" s="32">
         <v>6.7</v>
       </c>
     </row>
@@ -11163,7 +11870,7 @@
       <c r="A7" s="29">
         <v>60</v>
       </c>
-      <c r="B7" s="44">
+      <c r="B7" s="32">
         <v>5.55</v>
       </c>
     </row>
@@ -11171,7 +11878,7 @@
       <c r="A8" s="29">
         <v>80</v>
       </c>
-      <c r="B8" s="44">
+      <c r="B8" s="32">
         <v>4.42</v>
       </c>
     </row>
@@ -11179,7 +11886,7 @@
       <c r="A9" s="29">
         <v>100</v>
       </c>
-      <c r="B9" s="44">
+      <c r="B9" s="32">
         <v>3.71</v>
       </c>
     </row>
@@ -11187,7 +11894,7 @@
       <c r="A10" s="29">
         <v>120</v>
       </c>
-      <c r="B10" s="44">
+      <c r="B10" s="32">
         <v>3.05</v>
       </c>
     </row>
@@ -11195,7 +11902,7 @@
       <c r="A11" s="29">
         <v>140</v>
       </c>
-      <c r="B11" s="44">
+      <c r="B11" s="32">
         <v>2.5099999999999998</v>
       </c>
     </row>
@@ -11203,7 +11910,7 @@
       <c r="A12" s="29">
         <v>160</v>
       </c>
-      <c r="B12" s="44">
+      <c r="B12" s="32">
         <v>2.06</v>
       </c>
     </row>
@@ -11211,7 +11918,7 @@
       <c r="A13" s="29">
         <v>180</v>
       </c>
-      <c r="B13" s="44">
+      <c r="B13" s="32">
         <v>1.69</v>
       </c>
     </row>
@@ -11219,7 +11926,7 @@
       <c r="A14" s="29">
         <v>200</v>
       </c>
-      <c r="B14" s="44">
+      <c r="B14" s="32">
         <v>1.39</v>
       </c>
     </row>
@@ -11227,7 +11934,7 @@
       <c r="A15" s="29">
         <v>220</v>
       </c>
-      <c r="B15" s="44">
+      <c r="B15" s="32">
         <v>1.1399999999999999</v>
       </c>
     </row>
@@ -11235,7 +11942,7 @@
       <c r="A16" s="29">
         <v>240</v>
       </c>
-      <c r="B16" s="44">
+      <c r="B16" s="32">
         <v>0.93</v>
       </c>
     </row>
@@ -11243,7 +11950,7 @@
       <c r="A17" s="29">
         <v>260</v>
       </c>
-      <c r="B17" s="44">
+      <c r="B17" s="32">
         <v>0.77</v>
       </c>
     </row>
@@ -11251,7 +11958,7 @@
       <c r="A18" s="29">
         <v>280</v>
       </c>
-      <c r="B18" s="44">
+      <c r="B18" s="32">
         <v>0.63</v>
       </c>
     </row>
@@ -11259,7 +11966,7 @@
       <c r="A19" s="29">
         <v>300</v>
       </c>
-      <c r="B19" s="44">
+      <c r="B19" s="32">
         <v>0.52</v>
       </c>
     </row>
@@ -11267,7 +11974,7 @@
       <c r="A20" s="29">
         <v>320</v>
       </c>
-      <c r="B20" s="44">
+      <c r="B20" s="32">
         <v>0.43</v>
       </c>
     </row>
@@ -11275,7 +11982,7 @@
       <c r="A21" s="29">
         <v>340</v>
       </c>
-      <c r="B21" s="44">
+      <c r="B21" s="32">
         <v>0.35</v>
       </c>
     </row>
@@ -11283,7 +11990,7 @@
       <c r="A22" s="29">
         <v>360</v>
       </c>
-      <c r="B22" s="44">
+      <c r="B22" s="32">
         <v>0.28999999999999998</v>
       </c>
     </row>
@@ -11291,7 +11998,7 @@
       <c r="A23" s="29">
         <v>380</v>
       </c>
-      <c r="B23" s="44">
+      <c r="B23" s="32">
         <v>0.24</v>
       </c>
     </row>
@@ -11299,7 +12006,7 @@
       <c r="A24" s="29">
         <v>400</v>
       </c>
-      <c r="B24" s="44">
+      <c r="B24" s="32">
         <v>0.19</v>
       </c>
     </row>
@@ -11307,7 +12014,7 @@
       <c r="A25" s="29">
         <v>420</v>
       </c>
-      <c r="B25" s="44">
+      <c r="B25" s="32">
         <v>0.16</v>
       </c>
     </row>
@@ -11315,7 +12022,7 @@
       <c r="A26" s="29">
         <v>440</v>
       </c>
-      <c r="B26" s="44">
+      <c r="B26" s="32">
         <v>0.13</v>
       </c>
     </row>
@@ -11323,7 +12030,7 @@
       <c r="A27" s="29">
         <v>460</v>
       </c>
-      <c r="B27" s="44">
+      <c r="B27" s="32">
         <v>0.11</v>
       </c>
     </row>
@@ -11331,7 +12038,7 @@
       <c r="A28" s="29">
         <v>480</v>
       </c>
-      <c r="B28" s="44">
+      <c r="B28" s="32">
         <v>0.09</v>
       </c>
     </row>
@@ -11339,7 +12046,7 @@
       <c r="A29" s="29">
         <v>500</v>
       </c>
-      <c r="B29" s="44">
+      <c r="B29" s="32">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>

</xml_diff>